<commit_message>
Ver7 Formato para Versionamiento
</commit_message>
<xml_diff>
--- a/Libro Dominio Infraestructura Urbana.xlsx
+++ b/Libro Dominio Infraestructura Urbana.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmp\Documents\DMQ\Excel to HTML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F641E6-37B7-404E-9071-D98BBDC3B70C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9DC5BA-F646-42A9-96AC-6A9E1475B5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Índice" sheetId="9" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="199">
   <si>
     <t>Dominio de Infraestructura Urbana</t>
   </si>
@@ -627,13 +627,31 @@
     <t>6. Actas de Reunión de Dominio</t>
   </si>
   <si>
-    <t>SAS</t>
-  </si>
-  <si>
-    <t>ASD</t>
-  </si>
-  <si>
-    <t>S</t>
+    <t>Normativa</t>
+  </si>
+  <si>
+    <t>Regla de calidad</t>
+  </si>
+  <si>
+    <t>Eliminación</t>
+  </si>
+  <si>
+    <t>Proyecto</t>
+  </si>
+  <si>
+    <t>Lista Referencia</t>
+  </si>
+  <si>
+    <t>Dominio Externo</t>
+  </si>
+  <si>
+    <t>Creación</t>
+  </si>
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>Término</t>
   </si>
 </sst>
 </file>
@@ -641,12 +659,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.000%"/>
-    <numFmt numFmtId="166" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="167" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.000%"/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="52">
+  <fonts count="55">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -793,12 +811,6 @@
     </font>
     <font>
       <sz val="5"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -964,6 +976,32 @@
       <sz val="10"/>
       <name val="Roboto Ligth"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="13">
     <fill>
@@ -1039,7 +1077,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="95">
+  <borders count="101">
     <border>
       <left/>
       <right/>
@@ -2269,15 +2307,79 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="271">
+  <cellXfs count="296">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2326,15 +2428,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2344,7 +2439,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2391,18 +2485,6 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2412,63 +2494,63 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="34" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="34" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2502,55 +2584,55 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="43" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="35" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="36" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="7" borderId="56" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="31" fillId="7" borderId="56" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="60" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2565,13 +2647,13 @@
     <xf numFmtId="10" fontId="4" fillId="0" borderId="60" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="41" fillId="0" borderId="44" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="20" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="40" fillId="0" borderId="44" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="20" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2586,7 +2668,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="20" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2604,13 +2686,13 @@
     <xf numFmtId="10" fontId="4" fillId="0" borderId="65" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="41" fillId="0" borderId="66" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="20" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="40" fillId="0" borderId="66" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="20" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2626,25 +2708,25 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="5" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="5" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2656,16 +2738,16 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="30" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="80" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="80" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2674,7 +2756,7 @@
     <xf numFmtId="10" fontId="4" fillId="0" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="42" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="41" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2698,16 +2780,16 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="48" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="84" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="85" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="84" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="85" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="84" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2716,7 +2798,7 @@
     <xf numFmtId="10" fontId="4" fillId="0" borderId="86" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="42" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="41" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="48" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2782,7 +2864,7 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="60" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2827,20 +2909,20 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="59" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="60" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="64" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="65" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="59" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="60" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="64" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="65" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="60" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2883,136 +2965,143 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="5" borderId="50" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="5" borderId="51" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="5" borderId="50" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="93" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="91" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="60" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="46" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="5" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="5" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="5" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="31" fillId="5" borderId="50" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="31" fillId="5" borderId="51" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="5" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="5" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="5" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="5" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="5" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="5" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="5" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="5" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="5" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="31" fillId="5" borderId="50" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="5" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="93" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="91" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="60" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="46" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="5" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3021,6 +3110,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="95" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="96" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3032,14 +3139,66 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="65" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="4" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="52" fillId="4" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="4" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="53" fillId="4" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="4" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="4" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="52" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="53" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="4" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="52" fillId="4" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="4" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="53" fillId="4" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="4" builtinId="8"/>
+    <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -3051,6 +3210,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF7A2BAB"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -4775,7 +4939,7 @@
       <selection activeCell="G6" sqref="G6:N6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1"/>
   <cols>
     <col min="1" max="1" width="11.28515625" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1" collapsed="1"/>
@@ -4790,256 +4954,256 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="C1" s="250"/>
-      <c r="D1" s="250"/>
-      <c r="E1" s="250"/>
-      <c r="F1" s="250"/>
-      <c r="G1" s="250"/>
-      <c r="H1" s="250"/>
-      <c r="I1" s="250"/>
-      <c r="J1" s="250"/>
-      <c r="K1" s="250"/>
+      <c r="C1" s="239"/>
+      <c r="D1" s="239"/>
+      <c r="E1" s="239"/>
+      <c r="F1" s="239"/>
+      <c r="G1" s="239"/>
+      <c r="H1" s="239"/>
+      <c r="I1" s="239"/>
+      <c r="J1" s="239"/>
+      <c r="K1" s="239"/>
     </row>
     <row r="2" spans="1:17" ht="30">
-      <c r="A2" s="266"/>
-      <c r="B2" s="266"/>
-      <c r="C2" s="266"/>
-      <c r="D2" s="251"/>
-      <c r="E2" s="251"/>
-      <c r="F2" s="252" t="s">
+      <c r="A2" s="261"/>
+      <c r="B2" s="261"/>
+      <c r="C2" s="261"/>
+      <c r="D2" s="240"/>
+      <c r="E2" s="240"/>
+      <c r="F2" s="241" t="s">
         <v>181</v>
       </c>
-      <c r="G2" s="251"/>
-      <c r="H2" s="251"/>
-      <c r="I2" s="251"/>
-      <c r="J2" s="251"/>
-      <c r="K2" s="251"/>
-      <c r="L2" s="251"/>
+      <c r="G2" s="240"/>
+      <c r="H2" s="240"/>
+      <c r="I2" s="240"/>
+      <c r="J2" s="240"/>
+      <c r="K2" s="240"/>
+      <c r="L2" s="240"/>
     </row>
     <row r="3" spans="1:17" ht="22.5" customHeight="1"/>
     <row r="4" spans="1:17" ht="14.25" customHeight="1">
-      <c r="G4" s="263" t="s">
+      <c r="G4" s="258" t="s">
         <v>182</v>
       </c>
-      <c r="H4" s="263"/>
-      <c r="I4" s="263"/>
-      <c r="J4" s="263"/>
-      <c r="K4" s="263"/>
-      <c r="L4" s="263"/>
-      <c r="M4" s="263"/>
-      <c r="N4" s="263"/>
-      <c r="O4" s="254"/>
-      <c r="P4" s="254"/>
-      <c r="Q4" s="254"/>
+      <c r="H4" s="258"/>
+      <c r="I4" s="258"/>
+      <c r="J4" s="258"/>
+      <c r="K4" s="258"/>
+      <c r="L4" s="258"/>
+      <c r="M4" s="258"/>
+      <c r="N4" s="258"/>
+      <c r="O4" s="243"/>
+      <c r="P4" s="243"/>
+      <c r="Q4" s="243"/>
     </row>
     <row r="5" spans="1:17" ht="7.5" customHeight="1">
-      <c r="G5" s="255"/>
-      <c r="H5" s="253"/>
-      <c r="I5" s="253"/>
-      <c r="J5" s="253"/>
-      <c r="K5" s="253"/>
-      <c r="L5" s="253"/>
-      <c r="M5" s="253"/>
-      <c r="N5" s="253"/>
-      <c r="O5" s="254"/>
-      <c r="P5" s="254"/>
-      <c r="Q5" s="254"/>
+      <c r="G5" s="244"/>
+      <c r="H5" s="242"/>
+      <c r="I5" s="242"/>
+      <c r="J5" s="242"/>
+      <c r="K5" s="242"/>
+      <c r="L5" s="242"/>
+      <c r="M5" s="242"/>
+      <c r="N5" s="242"/>
+      <c r="O5" s="243"/>
+      <c r="P5" s="243"/>
+      <c r="Q5" s="243"/>
     </row>
     <row r="6" spans="1:17" ht="13.5" customHeight="1">
-      <c r="G6" s="263" t="s">
+      <c r="G6" s="258" t="s">
         <v>183</v>
       </c>
-      <c r="H6" s="263"/>
-      <c r="I6" s="263"/>
-      <c r="J6" s="263"/>
-      <c r="K6" s="263"/>
-      <c r="L6" s="263"/>
-      <c r="M6" s="263"/>
-      <c r="N6" s="263"/>
-      <c r="O6" s="254"/>
-      <c r="P6" s="254"/>
-      <c r="Q6" s="254"/>
+      <c r="H6" s="258"/>
+      <c r="I6" s="258"/>
+      <c r="J6" s="258"/>
+      <c r="K6" s="258"/>
+      <c r="L6" s="258"/>
+      <c r="M6" s="258"/>
+      <c r="N6" s="258"/>
+      <c r="O6" s="243"/>
+      <c r="P6" s="243"/>
+      <c r="Q6" s="243"/>
     </row>
     <row r="7" spans="1:17" ht="7.5" customHeight="1">
-      <c r="G7" s="263"/>
-      <c r="H7" s="263"/>
-      <c r="I7" s="263"/>
-      <c r="J7" s="263"/>
-      <c r="K7" s="263"/>
-      <c r="L7" s="263"/>
-      <c r="M7" s="263"/>
-      <c r="N7" s="263"/>
-      <c r="O7" s="254"/>
-      <c r="P7" s="254"/>
-      <c r="Q7" s="254"/>
+      <c r="G7" s="258"/>
+      <c r="H7" s="258"/>
+      <c r="I7" s="258"/>
+      <c r="J7" s="258"/>
+      <c r="K7" s="258"/>
+      <c r="L7" s="258"/>
+      <c r="M7" s="258"/>
+      <c r="N7" s="258"/>
+      <c r="O7" s="243"/>
+      <c r="P7" s="243"/>
+      <c r="Q7" s="243"/>
     </row>
     <row r="8" spans="1:17" ht="15" customHeight="1">
-      <c r="G8" s="263" t="s">
+      <c r="G8" s="258" t="s">
         <v>184</v>
       </c>
-      <c r="H8" s="263"/>
-      <c r="I8" s="263"/>
-      <c r="J8" s="263"/>
-      <c r="K8" s="263"/>
-      <c r="L8" s="263"/>
-      <c r="M8" s="263"/>
-      <c r="N8" s="263"/>
-      <c r="O8" s="254"/>
-      <c r="P8" s="254"/>
-      <c r="Q8" s="254"/>
+      <c r="H8" s="258"/>
+      <c r="I8" s="258"/>
+      <c r="J8" s="258"/>
+      <c r="K8" s="258"/>
+      <c r="L8" s="258"/>
+      <c r="M8" s="258"/>
+      <c r="N8" s="258"/>
+      <c r="O8" s="243"/>
+      <c r="P8" s="243"/>
+      <c r="Q8" s="243"/>
     </row>
     <row r="9" spans="1:17" ht="2.25" customHeight="1">
-      <c r="G9" s="256">
+      <c r="G9" s="245">
         <v>5</v>
       </c>
-      <c r="H9" s="256"/>
-      <c r="I9" s="256"/>
-      <c r="J9" s="256"/>
-      <c r="K9" s="256"/>
-      <c r="L9" s="256"/>
-      <c r="M9" s="256"/>
-      <c r="N9" s="256"/>
-      <c r="O9" s="254"/>
-      <c r="P9" s="254"/>
-      <c r="Q9" s="254"/>
+      <c r="H9" s="245"/>
+      <c r="I9" s="245"/>
+      <c r="J9" s="245"/>
+      <c r="K9" s="245"/>
+      <c r="L9" s="245"/>
+      <c r="M9" s="245"/>
+      <c r="N9" s="245"/>
+      <c r="O9" s="243"/>
+      <c r="P9" s="243"/>
+      <c r="Q9" s="243"/>
     </row>
     <row r="10" spans="1:17" ht="16.5" customHeight="1">
-      <c r="G10" s="264" t="s">
+      <c r="G10" s="259" t="s">
         <v>185</v>
       </c>
-      <c r="H10" s="264"/>
-      <c r="I10" s="253"/>
-      <c r="J10" s="253"/>
-      <c r="K10" s="253"/>
-      <c r="L10" s="253"/>
-      <c r="M10" s="253"/>
-      <c r="N10" s="253"/>
-      <c r="O10" s="254"/>
-      <c r="P10" s="254"/>
-      <c r="Q10" s="254"/>
+      <c r="H10" s="259"/>
+      <c r="I10" s="242"/>
+      <c r="J10" s="242"/>
+      <c r="K10" s="242"/>
+      <c r="L10" s="242"/>
+      <c r="M10" s="242"/>
+      <c r="N10" s="242"/>
+      <c r="O10" s="243"/>
+      <c r="P10" s="243"/>
+      <c r="Q10" s="243"/>
     </row>
     <row r="11" spans="1:17" ht="16.5" hidden="1" customHeight="1">
-      <c r="G11" s="257" t="s">
+      <c r="G11" s="246" t="s">
         <v>186</v>
       </c>
-      <c r="H11" s="253"/>
-      <c r="I11" s="253"/>
-      <c r="J11" s="253"/>
-      <c r="K11" s="253"/>
-      <c r="L11" s="253"/>
-      <c r="M11" s="253"/>
-      <c r="N11" s="253"/>
-      <c r="O11" s="254"/>
-      <c r="P11" s="254"/>
-      <c r="Q11" s="254"/>
+      <c r="H11" s="242"/>
+      <c r="I11" s="242"/>
+      <c r="J11" s="242"/>
+      <c r="K11" s="242"/>
+      <c r="L11" s="242"/>
+      <c r="M11" s="242"/>
+      <c r="N11" s="242"/>
+      <c r="O11" s="243"/>
+      <c r="P11" s="243"/>
+      <c r="Q11" s="243"/>
     </row>
     <row r="12" spans="1:17" ht="7.5" customHeight="1">
-      <c r="G12" s="255"/>
-      <c r="H12" s="253"/>
-      <c r="I12" s="253"/>
-      <c r="J12" s="253"/>
-      <c r="K12" s="253"/>
-      <c r="L12" s="253"/>
-      <c r="M12" s="253"/>
-      <c r="N12" s="253"/>
-      <c r="O12" s="254"/>
-      <c r="P12" s="254"/>
-      <c r="Q12" s="254"/>
+      <c r="G12" s="244"/>
+      <c r="H12" s="242"/>
+      <c r="I12" s="242"/>
+      <c r="J12" s="242"/>
+      <c r="K12" s="242"/>
+      <c r="L12" s="242"/>
+      <c r="M12" s="242"/>
+      <c r="N12" s="242"/>
+      <c r="O12" s="243"/>
+      <c r="P12" s="243"/>
+      <c r="Q12" s="243"/>
     </row>
     <row r="13" spans="1:17" ht="15" customHeight="1">
-      <c r="G13" s="263" t="s">
+      <c r="G13" s="258" t="s">
         <v>187</v>
       </c>
-      <c r="H13" s="263"/>
-      <c r="I13" s="263"/>
-      <c r="J13" s="263"/>
-      <c r="K13" s="263"/>
-      <c r="L13" s="263"/>
-      <c r="M13" s="263"/>
-      <c r="N13" s="263"/>
-      <c r="O13" s="258"/>
-      <c r="P13" s="258"/>
-      <c r="Q13" s="258"/>
+      <c r="H13" s="258"/>
+      <c r="I13" s="258"/>
+      <c r="J13" s="258"/>
+      <c r="K13" s="258"/>
+      <c r="L13" s="258"/>
+      <c r="M13" s="258"/>
+      <c r="N13" s="258"/>
+      <c r="O13" s="247"/>
+      <c r="P13" s="247"/>
+      <c r="Q13" s="247"/>
     </row>
     <row r="14" spans="1:17" ht="18" customHeight="1">
-      <c r="G14" s="264" t="s">
+      <c r="G14" s="259" t="s">
         <v>185</v>
       </c>
-      <c r="H14" s="264"/>
-      <c r="I14" s="259"/>
-      <c r="J14" s="259"/>
-      <c r="K14" s="259"/>
-      <c r="L14" s="259"/>
-      <c r="M14" s="259"/>
-      <c r="N14" s="259"/>
-      <c r="O14" s="260"/>
-      <c r="P14" s="260"/>
-      <c r="Q14" s="260"/>
+      <c r="H14" s="259"/>
+      <c r="I14" s="248"/>
+      <c r="J14" s="248"/>
+      <c r="K14" s="248"/>
+      <c r="L14" s="248"/>
+      <c r="M14" s="248"/>
+      <c r="N14" s="248"/>
+      <c r="O14" s="249"/>
+      <c r="P14" s="249"/>
+      <c r="Q14" s="249"/>
     </row>
     <row r="15" spans="1:17" ht="7.5" customHeight="1">
-      <c r="G15" s="257"/>
-      <c r="H15" s="253"/>
-      <c r="I15" s="253"/>
-      <c r="J15" s="253"/>
-      <c r="K15" s="253"/>
-      <c r="L15" s="253"/>
-      <c r="M15" s="253"/>
-      <c r="N15" s="253"/>
-      <c r="O15" s="254"/>
-      <c r="P15" s="254"/>
-      <c r="Q15" s="254"/>
+      <c r="G15" s="246"/>
+      <c r="H15" s="242"/>
+      <c r="I15" s="242"/>
+      <c r="J15" s="242"/>
+      <c r="K15" s="242"/>
+      <c r="L15" s="242"/>
+      <c r="M15" s="242"/>
+      <c r="N15" s="242"/>
+      <c r="O15" s="243"/>
+      <c r="P15" s="243"/>
+      <c r="Q15" s="243"/>
     </row>
     <row r="16" spans="1:17" ht="17.25" customHeight="1">
-      <c r="G16" s="263" t="s">
+      <c r="G16" s="258" t="s">
         <v>188</v>
       </c>
-      <c r="H16" s="263"/>
-      <c r="I16" s="263"/>
-      <c r="J16" s="263"/>
-      <c r="K16" s="263"/>
-      <c r="L16" s="263"/>
-      <c r="M16" s="263"/>
-      <c r="N16" s="263"/>
-      <c r="O16" s="254"/>
-      <c r="P16" s="254"/>
-      <c r="Q16" s="254"/>
+      <c r="H16" s="258"/>
+      <c r="I16" s="258"/>
+      <c r="J16" s="258"/>
+      <c r="K16" s="258"/>
+      <c r="L16" s="258"/>
+      <c r="M16" s="258"/>
+      <c r="N16" s="258"/>
+      <c r="O16" s="243"/>
+      <c r="P16" s="243"/>
+      <c r="Q16" s="243"/>
     </row>
     <row r="17" spans="7:20" ht="17.25" customHeight="1">
-      <c r="G17" s="263" t="s">
+      <c r="G17" s="258" t="s">
         <v>189</v>
       </c>
-      <c r="H17" s="263"/>
-      <c r="I17" s="263"/>
-      <c r="J17" s="263"/>
-      <c r="K17" s="263"/>
-      <c r="L17" s="263"/>
-      <c r="M17" s="263"/>
-      <c r="N17" s="263"/>
-      <c r="O17" s="254"/>
-      <c r="P17" s="254"/>
-      <c r="Q17" s="254"/>
+      <c r="H17" s="258"/>
+      <c r="I17" s="258"/>
+      <c r="J17" s="258"/>
+      <c r="K17" s="258"/>
+      <c r="L17" s="258"/>
+      <c r="M17" s="258"/>
+      <c r="N17" s="258"/>
+      <c r="O17" s="243"/>
+      <c r="P17" s="243"/>
+      <c r="Q17" s="243"/>
     </row>
     <row r="18" spans="7:20" ht="17.25" customHeight="1">
-      <c r="G18" s="261"/>
-      <c r="H18" s="261"/>
-      <c r="I18" s="259"/>
-      <c r="J18" s="259"/>
-      <c r="K18" s="259"/>
-      <c r="L18" s="259"/>
-      <c r="M18" s="259"/>
-      <c r="N18" s="259"/>
-      <c r="O18" s="254"/>
-      <c r="P18" s="254"/>
-      <c r="Q18" s="254"/>
+      <c r="G18" s="250"/>
+      <c r="H18" s="250"/>
+      <c r="I18" s="248"/>
+      <c r="J18" s="248"/>
+      <c r="K18" s="248"/>
+      <c r="L18" s="248"/>
+      <c r="M18" s="248"/>
+      <c r="N18" s="248"/>
+      <c r="O18" s="243"/>
+      <c r="P18" s="243"/>
+      <c r="Q18" s="243"/>
     </row>
     <row r="19" spans="7:20"/>
-    <row r="20" spans="7:20" s="262" customFormat="1" ht="3.75" customHeight="1"/>
+    <row r="20" spans="7:20" s="251" customFormat="1" ht="3.75" customHeight="1"/>
     <row r="21" spans="7:20" ht="12.75" customHeight="1">
-      <c r="P21" s="265"/>
-      <c r="Q21" s="265"/>
-      <c r="R21" s="265"/>
-      <c r="S21" s="265"/>
-      <c r="T21" s="265"/>
+      <c r="P21" s="260"/>
+      <c r="Q21" s="260"/>
+      <c r="R21" s="260"/>
+      <c r="S21" s="260"/>
+      <c r="T21" s="260"/>
     </row>
     <row r="22" spans="7:20"/>
     <row r="23" spans="7:20"/>
@@ -5089,11 +5253,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:XDQ66"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C23" sqref="B23:C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.25" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25" zeroHeight="1"/>
   <cols>
     <col min="1" max="1" width="18.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="76" style="1" customWidth="1"/>
@@ -5109,7 +5273,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1"/>
     <row r="2" spans="1:7" ht="60">
-      <c r="B2" s="205" t="s">
+      <c r="B2" s="197" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2"/>
@@ -5123,7 +5287,7 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="205"/>
+      <c r="G3" s="197"/>
     </row>
     <row r="4" spans="1:7" ht="30">
       <c r="B4" s="3"/>
@@ -5131,7 +5295,7 @@
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="205"/>
+      <c r="G4" s="197"/>
     </row>
     <row r="5" spans="1:7" ht="14.45" customHeight="1">
       <c r="B5" s="3"/>
@@ -5143,34 +5307,34 @@
     </row>
     <row r="6" spans="1:7" ht="19.5" customHeight="1"/>
     <row r="7" spans="1:7" ht="27" customHeight="1">
-      <c r="B7" s="213" t="s">
+      <c r="B7" s="205" t="s">
         <v>172</v>
       </c>
-      <c r="D7" s="214"/>
-      <c r="E7" s="213"/>
-      <c r="F7" s="213"/>
-      <c r="G7" s="213"/>
+      <c r="D7" s="206"/>
+      <c r="E7" s="205"/>
+      <c r="F7" s="205"/>
+      <c r="G7" s="205"/>
     </row>
     <row r="8" spans="1:7" ht="24" customHeight="1"/>
     <row r="9" spans="1:7">
-      <c r="B9" s="216" t="s">
+      <c r="B9" s="208" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="215"/>
-      <c r="D9" s="215"/>
-      <c r="E9" s="215"/>
-      <c r="F9" s="215"/>
-      <c r="G9" s="215"/>
+      <c r="C9" s="207"/>
+      <c r="D9" s="207"/>
+      <c r="E9" s="207"/>
+      <c r="F9" s="207"/>
+      <c r="G9" s="207"/>
     </row>
     <row r="10" spans="1:7"/>
     <row r="11" spans="1:7" ht="23.25">
-      <c r="B11" s="214" t="s">
+      <c r="B11" s="206" t="s">
         <v>173</v>
       </c>
-      <c r="D11" s="214"/>
-      <c r="E11" s="214"/>
-      <c r="F11" s="214"/>
-      <c r="G11" s="214"/>
+      <c r="D11" s="206"/>
+      <c r="E11" s="206"/>
+      <c r="F11" s="206"/>
+      <c r="G11" s="206"/>
     </row>
     <row r="12" spans="1:7"/>
     <row r="13" spans="1:7">
@@ -5181,13 +5345,13 @@
     <row r="14" spans="1:7"/>
     <row r="15" spans="1:7" ht="37.5" customHeight="1"/>
     <row r="16" spans="1:7" ht="27.75" customHeight="1">
-      <c r="A16" s="192" t="s">
+      <c r="A16" s="184" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="192" t="s">
+      <c r="B16" s="184" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="194" t="s">
+      <c r="C16" s="186" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="4" t="s">
@@ -5196,12 +5360,12 @@
       <c r="E16" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="195" t="s">
+      <c r="F16" s="187" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="48.75" customHeight="1">
-      <c r="A17" s="193" t="s">
+      <c r="A17" s="185" t="s">
         <v>9</v>
       </c>
       <c r="B17" s="6" t="s">
@@ -5224,20 +5388,20 @@
     <row r="19" spans="1:6" ht="18.75" customHeight="1"/>
     <row r="20" spans="1:6" ht="35.25" customHeight="1"/>
     <row r="21" spans="1:6" ht="28.5" customHeight="1">
-      <c r="B21" s="214" t="s">
+      <c r="B21" s="206" t="s">
         <v>174</v>
       </c>
-      <c r="D21" s="214"/>
+      <c r="D21" s="206"/>
     </row>
     <row r="22" spans="1:6" s="8" customFormat="1" ht="42.75" customHeight="1">
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
     </row>
     <row r="23" spans="1:6" s="8" customFormat="1" ht="36" customHeight="1">
-      <c r="A23" s="208" t="s">
+      <c r="A23" s="200" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="212" t="s">
+      <c r="B23" s="204" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="10" t="s">
@@ -5245,137 +5409,137 @@
       </c>
     </row>
     <row r="24" spans="1:6" s="12" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A24" s="211" t="s">
+      <c r="A24" s="203" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="193" t="s">
+      <c r="B24" s="185" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="193"/>
+      <c r="C24" s="185"/>
     </row>
     <row r="25" spans="1:6" s="12" customFormat="1" ht="40.5" customHeight="1">
-      <c r="A25" s="211" t="s">
+      <c r="A25" s="203" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="193" t="s">
+      <c r="B25" s="185" t="s">
         <v>19</v>
       </c>
       <c r="C25" s="11"/>
     </row>
     <row r="26" spans="1:6" s="12" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A26" s="211" t="s">
+      <c r="A26" s="203" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="193" t="s">
+      <c r="B26" s="185" t="s">
         <v>21</v>
       </c>
       <c r="C26" s="11"/>
     </row>
     <row r="27" spans="1:6" s="12" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A27" s="211" t="s">
+      <c r="A27" s="203" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="193" t="s">
+      <c r="B27" s="185" t="s">
         <v>23</v>
       </c>
       <c r="C27" s="11"/>
     </row>
     <row r="28" spans="1:6" s="12" customFormat="1" ht="40.5" customHeight="1">
-      <c r="A28" s="211" t="s">
+      <c r="A28" s="203" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="193" t="s">
+      <c r="B28" s="185" t="s">
         <v>25</v>
       </c>
       <c r="C28" s="11"/>
     </row>
     <row r="29" spans="1:6" s="12" customFormat="1" ht="24" customHeight="1">
-      <c r="A29" s="211" t="s">
+      <c r="A29" s="203" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="193" t="s">
+      <c r="B29" s="185" t="s">
         <v>27</v>
       </c>
       <c r="C29" s="11"/>
     </row>
     <row r="30" spans="1:6" s="12" customFormat="1" hidden="1">
-      <c r="A30" s="211"/>
-      <c r="B30" s="193"/>
+      <c r="A30" s="203"/>
+      <c r="B30" s="185"/>
       <c r="C30" s="11"/>
     </row>
     <row r="31" spans="1:6" s="12" customFormat="1" hidden="1">
-      <c r="A31" s="211"/>
-      <c r="B31" s="193"/>
+      <c r="A31" s="203"/>
+      <c r="B31" s="185"/>
       <c r="C31" s="11"/>
     </row>
     <row r="32" spans="1:6" s="12" customFormat="1" hidden="1">
-      <c r="A32" s="211"/>
-      <c r="B32" s="193"/>
+      <c r="A32" s="203"/>
+      <c r="B32" s="185"/>
       <c r="C32" s="11"/>
     </row>
     <row r="33" spans="1:4" s="12" customFormat="1" hidden="1">
-      <c r="A33" s="211"/>
-      <c r="B33" s="193"/>
+      <c r="A33" s="203"/>
+      <c r="B33" s="185"/>
       <c r="C33" s="11"/>
     </row>
     <row r="34" spans="1:4" s="12" customFormat="1" hidden="1">
-      <c r="A34" s="211"/>
-      <c r="B34" s="193"/>
+      <c r="A34" s="203"/>
+      <c r="B34" s="185"/>
       <c r="C34" s="11"/>
     </row>
     <row r="35" spans="1:4" s="12" customFormat="1" hidden="1">
-      <c r="A35" s="211"/>
-      <c r="B35" s="193"/>
+      <c r="A35" s="203"/>
+      <c r="B35" s="185"/>
       <c r="C35" s="11"/>
     </row>
     <row r="36" spans="1:4" s="12" customFormat="1" hidden="1">
-      <c r="A36" s="211"/>
-      <c r="B36" s="193"/>
+      <c r="A36" s="203"/>
+      <c r="B36" s="185"/>
       <c r="C36" s="11"/>
     </row>
     <row r="37" spans="1:4" s="12" customFormat="1" hidden="1">
-      <c r="A37" s="211"/>
-      <c r="B37" s="193"/>
+      <c r="A37" s="203"/>
+      <c r="B37" s="185"/>
       <c r="C37" s="11"/>
     </row>
     <row r="38" spans="1:4" s="12" customFormat="1" hidden="1">
-      <c r="A38" s="211"/>
-      <c r="B38" s="193"/>
+      <c r="A38" s="203"/>
+      <c r="B38" s="185"/>
       <c r="C38" s="11"/>
     </row>
     <row r="39" spans="1:4" s="12" customFormat="1" hidden="1">
-      <c r="A39" s="211"/>
-      <c r="B39" s="193"/>
+      <c r="A39" s="203"/>
+      <c r="B39" s="185"/>
       <c r="C39" s="11"/>
     </row>
     <row r="40" spans="1:4" s="12" customFormat="1" hidden="1">
-      <c r="A40" s="211"/>
-      <c r="B40" s="193"/>
+      <c r="A40" s="203"/>
+      <c r="B40" s="185"/>
       <c r="C40" s="11"/>
     </row>
     <row r="41" spans="1:4" s="12" customFormat="1" hidden="1">
-      <c r="A41" s="211"/>
-      <c r="B41" s="193"/>
+      <c r="A41" s="203"/>
+      <c r="B41" s="185"/>
       <c r="C41" s="11"/>
     </row>
     <row r="42" spans="1:4" s="12" customFormat="1" hidden="1">
-      <c r="A42" s="211"/>
-      <c r="B42" s="193"/>
+      <c r="A42" s="203"/>
+      <c r="B42" s="185"/>
       <c r="C42" s="11"/>
     </row>
     <row r="43" spans="1:4" s="12" customFormat="1" hidden="1">
-      <c r="A43" s="211"/>
-      <c r="B43" s="193"/>
+      <c r="A43" s="203"/>
+      <c r="B43" s="185"/>
       <c r="C43" s="11"/>
     </row>
     <row r="44" spans="1:4" s="12" customFormat="1" hidden="1">
-      <c r="A44" s="211"/>
-      <c r="B44" s="193"/>
+      <c r="A44" s="203"/>
+      <c r="B44" s="185"/>
       <c r="C44" s="11"/>
     </row>
     <row r="45" spans="1:4" s="12" customFormat="1" hidden="1">
-      <c r="A45" s="211"/>
-      <c r="B45" s="193"/>
+      <c r="A45" s="203"/>
+      <c r="B45" s="185"/>
       <c r="C45" s="11"/>
     </row>
     <row r="46" spans="1:4" s="12" customFormat="1" ht="36" customHeight="1">
@@ -5383,81 +5547,81 @@
       <c r="D46" s="13"/>
     </row>
     <row r="47" spans="1:4" s="8" customFormat="1" ht="29.25" customHeight="1">
-      <c r="B47" s="214" t="s">
+      <c r="B47" s="206" t="s">
         <v>171</v>
       </c>
-      <c r="D47" s="214"/>
+      <c r="D47" s="206"/>
     </row>
     <row r="48" spans="1:4" s="8" customFormat="1" ht="29.25" customHeight="1">
       <c r="C48" s="14"/>
       <c r="D48" s="14"/>
     </row>
     <row r="49" spans="1:4" s="8" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A49" s="210" t="s">
+      <c r="A49" s="295" t="s">
         <v>28</v>
       </c>
-      <c r="B49" s="210" t="s">
+      <c r="B49" s="295" t="s">
         <v>29</v>
       </c>
-      <c r="C49" s="210" t="s">
+      <c r="C49" s="295" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:4" s="8" customFormat="1" ht="72.75" customHeight="1">
-      <c r="A50" s="241" t="s">
+      <c r="A50" s="230" t="s">
         <v>31</v>
       </c>
-      <c r="B50" s="219" t="s">
+      <c r="B50" s="211" t="s">
         <v>32</v>
       </c>
-      <c r="C50" s="207" t="s">
+      <c r="C50" s="199" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="51" spans="1:4" s="8" customFormat="1" ht="72.75" customHeight="1">
-      <c r="A51" s="242"/>
-      <c r="B51" s="219" t="s">
+      <c r="A51" s="231"/>
+      <c r="B51" s="211" t="s">
         <v>34</v>
       </c>
-      <c r="C51" s="207" t="s">
+      <c r="C51" s="199" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="52" spans="1:4" s="8" customFormat="1" ht="72.75" customHeight="1">
-      <c r="A52" s="243"/>
-      <c r="B52" s="219" t="s">
+      <c r="A52" s="232"/>
+      <c r="B52" s="211" t="s">
         <v>35</v>
       </c>
-      <c r="C52" s="207" t="s">
+      <c r="C52" s="199" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="53" spans="1:4" s="8" customFormat="1" ht="48" customHeight="1">
-      <c r="A53" s="241" t="s">
+      <c r="A53" s="230" t="s">
         <v>37</v>
       </c>
-      <c r="B53" s="219" t="s">
+      <c r="B53" s="211" t="s">
         <v>38</v>
       </c>
-      <c r="C53" s="207" t="s">
+      <c r="C53" s="199" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="54" spans="1:4" s="8" customFormat="1" ht="48" customHeight="1">
-      <c r="A54" s="242"/>
-      <c r="B54" s="219" t="s">
+      <c r="A54" s="231"/>
+      <c r="B54" s="211" t="s">
         <v>40</v>
       </c>
-      <c r="C54" s="207" t="s">
+      <c r="C54" s="199" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:4" s="8" customFormat="1" ht="48" customHeight="1">
-      <c r="A55" s="243"/>
-      <c r="B55" s="219" t="s">
+      <c r="A55" s="232"/>
+      <c r="B55" s="211" t="s">
         <v>41</v>
       </c>
-      <c r="C55" s="207" t="s">
+      <c r="C55" s="199" t="s">
         <v>42</v>
       </c>
     </row>
@@ -5466,64 +5630,64 @@
       <c r="D56" s="13"/>
     </row>
     <row r="57" spans="1:4" s="8" customFormat="1" ht="29.25" customHeight="1">
-      <c r="B57" s="214" t="s">
+      <c r="B57" s="206" t="s">
         <v>43</v>
       </c>
-      <c r="D57" s="214"/>
+      <c r="D57" s="206"/>
     </row>
     <row r="58" spans="1:4" s="8" customFormat="1" ht="29.25" customHeight="1">
       <c r="C58" s="13"/>
       <c r="D58" s="13"/>
     </row>
     <row r="59" spans="1:4" s="8" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A59" s="210" t="s">
+      <c r="A59" s="202" t="s">
         <v>44</v>
       </c>
-      <c r="B59" s="206" t="s">
+      <c r="B59" s="198" t="s">
         <v>45</v>
       </c>
       <c r="C59" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D59" s="210"/>
+      <c r="D59" s="202"/>
     </row>
     <row r="60" spans="1:4" s="8" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A60" s="209" t="s">
+      <c r="A60" s="201" t="s">
         <v>46</v>
       </c>
-      <c r="B60" s="193" t="s">
+      <c r="B60" s="185" t="s">
         <v>47</v>
       </c>
       <c r="C60" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="D60" s="209" t="s">
+      <c r="D60" s="201" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="61" spans="1:4" s="8" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A61" s="209" t="s">
+      <c r="A61" s="201" t="s">
         <v>49</v>
       </c>
-      <c r="B61" s="193" t="s">
+      <c r="B61" s="185" t="s">
         <v>50</v>
       </c>
       <c r="C61" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="D61" s="209"/>
+      <c r="D61" s="201"/>
     </row>
     <row r="62" spans="1:4" s="8" customFormat="1" ht="73.5" customHeight="1">
-      <c r="A62" s="209" t="s">
+      <c r="A62" s="201" t="s">
         <v>51</v>
       </c>
-      <c r="B62" s="193" t="s">
+      <c r="B62" s="185" t="s">
         <v>52</v>
       </c>
       <c r="C62" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D62" s="209"/>
+      <c r="D62" s="201"/>
     </row>
     <row r="63" spans="1:4" s="8" customFormat="1" ht="29.25" customHeight="1">
       <c r="C63" s="13"/>
@@ -5538,19 +5702,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:R54"/>
+  <dimension ref="A1:R114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6:L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.25" customHeight="1" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.25" customHeight="1" zeroHeight="1"/>
   <cols>
     <col min="1" max="1" width="3.42578125" style="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="5.5703125" style="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="3.7109375" style="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="2.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.7109375" style="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="11.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" style="1" customWidth="1"/>
@@ -5568,289 +5732,414 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
-      <c r="A1" s="17"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
+      <c r="L1" s="272"/>
+      <c r="M1" s="272"/>
+      <c r="N1" s="272"/>
       <c r="O1" s="17"/>
       <c r="P1" s="17"/>
       <c r="Q1" s="17"/>
       <c r="R1" s="17"/>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
+      <c r="K2" s="252"/>
+      <c r="L2" s="272"/>
+      <c r="M2" s="272"/>
+      <c r="N2" s="272"/>
       <c r="O2" s="17"/>
       <c r="P2" s="17"/>
       <c r="Q2" s="17"/>
       <c r="R2" s="17"/>
     </row>
     <row r="3" spans="1:18" ht="30">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="17"/>
-      <c r="N3" s="19"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="253"/>
+      <c r="L3" s="272"/>
+      <c r="M3" s="272"/>
+      <c r="N3" s="273"/>
       <c r="O3" s="19"/>
       <c r="P3" s="19"/>
       <c r="Q3" s="19"/>
       <c r="R3" s="19"/>
     </row>
     <row r="4" spans="1:18" ht="30">
-      <c r="A4" s="17"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="F4" s="20" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="F4" s="254" t="s">
         <v>180</v>
       </c>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
+      <c r="G4" s="255"/>
+      <c r="H4" s="255"/>
+      <c r="I4" s="255"/>
+      <c r="J4" s="255"/>
+      <c r="K4" s="255"/>
+      <c r="L4" s="274"/>
+      <c r="M4" s="274"/>
+      <c r="N4" s="274"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
     </row>
     <row r="5" spans="1:18" ht="30">
-      <c r="A5" s="17"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-    </row>
-    <row r="6" spans="1:18" ht="30">
-      <c r="A6" s="17"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="221" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="L5" s="272"/>
+      <c r="M5" s="272"/>
+      <c r="N5" s="272"/>
+    </row>
+    <row r="6" spans="1:18" ht="15">
+      <c r="B6" s="256"/>
+      <c r="C6" s="256"/>
+      <c r="D6" s="256"/>
+      <c r="E6" s="280"/>
+      <c r="F6" s="281"/>
+      <c r="G6" s="281" t="s">
+        <v>198</v>
+      </c>
+      <c r="H6" s="282"/>
+      <c r="I6" s="283"/>
+      <c r="J6" s="283"/>
+      <c r="K6" s="281" t="s">
+        <v>197</v>
+      </c>
+      <c r="L6" s="284"/>
+      <c r="M6" s="272"/>
+      <c r="N6" s="272"/>
+    </row>
+    <row r="7" spans="1:18" ht="15">
+      <c r="B7" s="256"/>
+      <c r="C7" s="256"/>
+      <c r="D7" s="256"/>
+      <c r="E7" s="285"/>
+      <c r="F7" s="286" t="s">
+        <v>196</v>
+      </c>
+      <c r="G7" s="286" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="287"/>
+      <c r="I7" s="288"/>
+      <c r="J7" s="288"/>
+      <c r="K7" s="286" t="s">
+        <v>195</v>
+      </c>
+      <c r="L7" s="289"/>
+      <c r="M7" s="272"/>
+      <c r="N7" s="272"/>
+    </row>
+    <row r="8" spans="1:18" ht="15">
+      <c r="B8" s="256"/>
+      <c r="C8" s="256"/>
+      <c r="D8" s="256"/>
+      <c r="E8" s="285"/>
+      <c r="F8" s="286" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="286" t="s">
+        <v>194</v>
+      </c>
+      <c r="H8" s="287"/>
+      <c r="I8" s="288"/>
+      <c r="J8" s="288"/>
+      <c r="K8" s="286" t="s">
+        <v>193</v>
+      </c>
+      <c r="L8" s="289"/>
+      <c r="M8" s="272"/>
+      <c r="N8" s="272"/>
+    </row>
+    <row r="9" spans="1:18" ht="15">
+      <c r="B9" s="256"/>
+      <c r="C9" s="256"/>
+      <c r="D9" s="256"/>
+      <c r="E9" s="285"/>
+      <c r="F9" s="286" t="s">
+        <v>192</v>
+      </c>
+      <c r="G9" s="286" t="s">
+        <v>191</v>
+      </c>
+      <c r="H9" s="287"/>
+      <c r="I9" s="288"/>
+      <c r="J9" s="288"/>
+      <c r="K9" s="286" t="s">
+        <v>190</v>
+      </c>
+      <c r="L9" s="289"/>
+      <c r="M9" s="272"/>
+      <c r="N9" s="272"/>
+    </row>
+    <row r="10" spans="1:18" s="24" customFormat="1" ht="30.75" customHeight="1">
+      <c r="A10" s="1"/>
+      <c r="B10" s="256"/>
+      <c r="C10" s="256"/>
+      <c r="D10" s="256"/>
+      <c r="E10" s="290"/>
+      <c r="F10" s="291"/>
+      <c r="G10" s="291" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" s="292"/>
+      <c r="I10" s="293"/>
+      <c r="J10" s="293"/>
+      <c r="K10" s="291"/>
+      <c r="L10" s="294"/>
+      <c r="M10" s="275"/>
+      <c r="N10" s="276"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="25"/>
+    </row>
+    <row r="11" spans="1:18" s="24" customFormat="1" ht="30.75" customHeight="1" thickBot="1">
+      <c r="A11" s="1"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="257" t="s">
         <v>57</v>
       </c>
-      <c r="F6" s="22"/>
-    </row>
-    <row r="7" spans="1:18" ht="30">
-      <c r="A7" s="17"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-    </row>
-    <row r="8" spans="1:18" ht="30">
-      <c r="A8" s="17"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-    </row>
-    <row r="9" spans="1:18" ht="15" thickBot="1">
-      <c r="A9" s="17"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-    </row>
-    <row r="10" spans="1:18" s="27" customFormat="1" ht="30.75" thickBot="1">
-      <c r="A10" s="17"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="196" t="s">
+      <c r="F11" s="257"/>
+      <c r="G11" s="257"/>
+      <c r="H11" s="257"/>
+      <c r="I11" s="257"/>
+      <c r="J11" s="257"/>
+      <c r="K11" s="257"/>
+      <c r="L11" s="277"/>
+      <c r="M11" s="276"/>
+      <c r="N11" s="276"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="31"/>
+      <c r="R11" s="31"/>
+    </row>
+    <row r="12" spans="1:18" s="24" customFormat="1" ht="30.75" thickBot="1">
+      <c r="A12" s="17"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="188" t="s">
         <v>58</v>
       </c>
-      <c r="F10" s="25" t="s">
+      <c r="F12" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="G10" s="26" t="s">
+      <c r="G12" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="H10" s="25" t="s">
+      <c r="H12" s="266" t="s">
         <v>61</v>
       </c>
-      <c r="I10" s="26" t="s">
+      <c r="I12" s="267"/>
+      <c r="J12" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="J10" s="26" t="s">
+      <c r="K12" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="M10" s="28"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="29"/>
-      <c r="R10" s="29"/>
-    </row>
-    <row r="11" spans="1:18" s="27" customFormat="1" ht="30">
-      <c r="A11" s="17"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="30">
+      <c r="L12" s="276"/>
+      <c r="M12" s="276"/>
+      <c r="N12" s="278"/>
+      <c r="O12" s="37"/>
+      <c r="P12" s="37"/>
+      <c r="Q12" s="37"/>
+      <c r="R12" s="37"/>
+    </row>
+    <row r="13" spans="1:18" s="24" customFormat="1" ht="30">
+      <c r="A13" s="17"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="26">
         <v>1</v>
       </c>
-      <c r="F11" s="31" t="s">
+      <c r="F13" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="G11" s="32" t="s">
+      <c r="G13" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="H11" s="222"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="34" t="s">
+      <c r="H13" s="262"/>
+      <c r="I13" s="263"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="O11" s="35"/>
-      <c r="P11" s="35"/>
-      <c r="Q11" s="35"/>
-      <c r="R11" s="35"/>
-    </row>
-    <row r="12" spans="1:18" s="27" customFormat="1" ht="30">
-      <c r="A12" s="17"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="36">
+      <c r="L13" s="276"/>
+      <c r="M13" s="278"/>
+      <c r="N13" s="278"/>
+      <c r="O13" s="37"/>
+      <c r="P13" s="37"/>
+      <c r="Q13" s="37"/>
+      <c r="R13" s="37"/>
+    </row>
+    <row r="14" spans="1:18" ht="30">
+      <c r="A14" s="40"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="32">
         <v>2</v>
       </c>
-      <c r="F12" s="37" t="s">
+      <c r="F14" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="G12" s="38" t="s">
+      <c r="G14" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="H12" s="223"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="40" t="s">
+      <c r="H14" s="264"/>
+      <c r="I14" s="265"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L12" s="41"/>
-      <c r="M12" s="41"/>
-      <c r="N12" s="41"/>
-      <c r="O12" s="41"/>
-      <c r="P12" s="41"/>
-      <c r="Q12" s="41"/>
-      <c r="R12" s="41"/>
-    </row>
-    <row r="13" spans="1:18" s="27" customFormat="1" ht="30">
-      <c r="A13" s="17"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="43">
-        <v>3</v>
-      </c>
-      <c r="F13" s="42" t="s">
-        <v>190</v>
-      </c>
-      <c r="G13" s="43" t="s">
-        <v>191</v>
-      </c>
-      <c r="H13" s="42"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="42" t="s">
-        <v>192</v>
-      </c>
-      <c r="K13" s="18"/>
-      <c r="L13" s="41"/>
-      <c r="M13" s="41"/>
-      <c r="N13" s="41"/>
-      <c r="O13" s="41"/>
-      <c r="P13" s="41"/>
-      <c r="Q13" s="41"/>
-      <c r="R13" s="41"/>
-    </row>
-    <row r="14" spans="1:18" ht="18">
-      <c r="A14" s="44"/>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="46"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="46"/>
-      <c r="K14" s="48"/>
-      <c r="L14" s="44"/>
-      <c r="M14" s="44"/>
-      <c r="N14" s="44"/>
-      <c r="O14" s="44"/>
-      <c r="P14" s="44"/>
-      <c r="Q14" s="44"/>
+      <c r="L14" s="276"/>
+      <c r="M14" s="279"/>
+      <c r="N14" s="279"/>
+      <c r="O14" s="40"/>
+      <c r="P14" s="40"/>
+      <c r="Q14" s="40"/>
       <c r="R14" s="17"/>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" ht="30">
       <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="278"/>
+      <c r="M15" s="272"/>
+      <c r="N15" s="278"/>
     </row>
     <row r="16" spans="1:18">
       <c r="A16" s="17"/>
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="L16" s="272"/>
+      <c r="M16" s="272"/>
+      <c r="N16" s="272"/>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" s="17"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
-    </row>
-    <row r="18" spans="1:4" s="198" customFormat="1"/>
-    <row r="45"/>
-    <row r="46"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
-    <row r="49" ht="14.25" customHeight="1"/>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1"/>
-    <row r="52" ht="14.25" customHeight="1"/>
-    <row r="53" ht="14.25" customHeight="1"/>
-    <row r="54" ht="14.25" customHeight="1"/>
+      <c r="L17" s="272"/>
+      <c r="M17" s="272"/>
+      <c r="N17" s="272"/>
+    </row>
+    <row r="18" spans="1:14" s="190" customFormat="1"/>
+    <row r="33" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="34" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="35" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="36" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="37" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="38" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="39" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="40" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="41" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="42" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="43" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="44" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="45" s="1" customFormat="1"/>
+    <row r="46" s="1" customFormat="1"/>
+    <row r="47" s="1" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="48" s="1" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="49" s="1" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="50" s="1" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="51" s="1" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="52" s="1" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="53" s="1" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="54" s="1" customFormat="1" ht="14.25" customHeight="1"/>
+    <row r="55" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="56" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="57" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="58" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="59" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="60" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="61" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="62" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="63" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="64" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="65" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="66" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="67" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="68" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="69" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="70" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="71" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="72" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="73" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="74" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="75" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="76" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="77" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="78" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="79" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="80" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="81" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="82" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="83" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="84" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="85" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="86" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="87" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="88" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="89" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="90" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="91" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="92" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="93" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="94" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="95" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="96" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="97" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="98" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="99" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="100" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="101" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="102" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="103" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="104" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="105" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="106" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="107" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="108" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="109" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="110" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="111" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="112" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="113" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
+    <row r="114" s="1" customFormat="1" ht="14.25" hidden="1" customHeight="1"/>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H12:I12"/>
+  </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F11:F12" xr:uid="{00000000-0002-0000-0200-000001000000}">
-      <formula1>#REF!</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K13:K14" xr:uid="{AEF9AEF0-7BD2-424E-AB8F-4A135D71F9C2}">
+      <formula1>$K$3:$K$7</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G11:G12" xr:uid="{00000000-0002-0000-0200-000000000000}">
-      <formula1>$G$4:$G$4</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F13:F14" xr:uid="{A4925934-4A99-49F1-9EEB-550A913793B3}">
+      <formula1>$F$5:$F$7</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J11:J12" xr:uid="{00000000-0002-0000-0200-000002000000}">
-      <formula1>$K$3:$K$4</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G13:G14" xr:uid="{F7A27BE1-647B-4374-A1D3-76DC6393EC8E}">
+      <formula1>$G$4:$G$8</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5866,411 +6155,411 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="52" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" style="52" customWidth="1"/>
-    <col min="3" max="3" width="35.5703125" style="52" customWidth="1"/>
-    <col min="4" max="4" width="76.28515625" style="53" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="52" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" style="52" customWidth="1"/>
-    <col min="7" max="7" width="28.42578125" style="52" customWidth="1"/>
-    <col min="8" max="8" width="29.7109375" style="52" customWidth="1"/>
-    <col min="9" max="9" width="114.7109375" style="52" customWidth="1"/>
-    <col min="10" max="10" width="34.7109375" style="52" customWidth="1"/>
-    <col min="11" max="11" width="39" style="52" customWidth="1"/>
-    <col min="12" max="12" width="55.140625" style="52" customWidth="1"/>
-    <col min="13" max="13" width="36.5703125" style="52" customWidth="1"/>
-    <col min="14" max="14" width="29.140625" style="52" customWidth="1"/>
-    <col min="15" max="15" width="27.28515625" style="52" customWidth="1"/>
-    <col min="16" max="16" width="15.28515625" style="52" customWidth="1"/>
-    <col min="17" max="18" width="13.5703125" style="52" customWidth="1"/>
-    <col min="19" max="19" width="9.140625" style="52" customWidth="1"/>
-    <col min="20" max="85" width="0" style="52" hidden="1" customWidth="1"/>
-    <col min="86" max="16384" width="9.140625" style="52" hidden="1"/>
+    <col min="1" max="1" width="3.85546875" style="44" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" style="44" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" style="44" customWidth="1"/>
+    <col min="4" max="4" width="76.28515625" style="45" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="44" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" style="44" customWidth="1"/>
+    <col min="7" max="7" width="28.42578125" style="44" customWidth="1"/>
+    <col min="8" max="8" width="29.7109375" style="44" customWidth="1"/>
+    <col min="9" max="9" width="114.7109375" style="44" customWidth="1"/>
+    <col min="10" max="10" width="34.7109375" style="44" customWidth="1"/>
+    <col min="11" max="11" width="39" style="44" customWidth="1"/>
+    <col min="12" max="12" width="55.140625" style="44" customWidth="1"/>
+    <col min="13" max="13" width="36.5703125" style="44" customWidth="1"/>
+    <col min="14" max="14" width="29.140625" style="44" customWidth="1"/>
+    <col min="15" max="15" width="27.28515625" style="44" customWidth="1"/>
+    <col min="16" max="16" width="15.28515625" style="44" customWidth="1"/>
+    <col min="17" max="18" width="13.5703125" style="44" customWidth="1"/>
+    <col min="19" max="19" width="9.140625" style="44" customWidth="1"/>
+    <col min="20" max="85" width="0" style="44" hidden="1" customWidth="1"/>
+    <col min="86" max="16384" width="9.140625" style="44" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="24.75" customHeight="1"/>
     <row r="2" spans="2:18" ht="33.75" customHeight="1">
-      <c r="D2" s="54"/>
+      <c r="D2" s="46"/>
     </row>
     <row r="3" spans="2:18" ht="56.25" customHeight="1">
-      <c r="D3" s="220" t="s">
+      <c r="D3" s="212" t="s">
         <v>177</v>
       </c>
-      <c r="E3" s="220"/>
-      <c r="F3" s="220"/>
-      <c r="G3" s="220"/>
+      <c r="E3" s="212"/>
+      <c r="F3" s="212"/>
+      <c r="G3" s="212"/>
     </row>
     <row r="4" spans="2:18" ht="17.25" customHeight="1">
-      <c r="D4" s="52"/>
-      <c r="F4" s="55"/>
+      <c r="D4" s="44"/>
+      <c r="F4" s="47"/>
     </row>
     <row r="5" spans="2:18" ht="17.25" customHeight="1">
-      <c r="D5" s="52"/>
-      <c r="F5" s="55"/>
+      <c r="D5" s="44"/>
+      <c r="F5" s="47"/>
     </row>
     <row r="6" spans="2:18" ht="17.25" customHeight="1">
-      <c r="D6" s="52"/>
-      <c r="F6" s="55"/>
+      <c r="D6" s="44"/>
+      <c r="F6" s="47"/>
     </row>
     <row r="7" spans="2:18" ht="21" customHeight="1" thickBot="1"/>
     <row r="8" spans="2:18" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B8" s="217" t="s">
+      <c r="B8" s="209" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="217"/>
-      <c r="D8" s="218"/>
-      <c r="E8" s="182" t="s">
+      <c r="C8" s="209"/>
+      <c r="D8" s="210"/>
+      <c r="E8" s="174" t="s">
         <v>66</v>
       </c>
-      <c r="F8" s="182"/>
-      <c r="G8" s="197" t="s">
+      <c r="F8" s="174"/>
+      <c r="G8" s="189" t="s">
         <v>67</v>
       </c>
-      <c r="H8" s="56"/>
-      <c r="I8" s="57" t="s">
+      <c r="H8" s="48"/>
+      <c r="I8" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="J8" s="57"/>
-      <c r="K8" s="58"/>
-      <c r="L8" s="58"/>
-      <c r="M8" s="58"/>
-      <c r="N8" s="58"/>
-      <c r="O8" s="58"/>
-      <c r="P8" s="58"/>
-      <c r="Q8" s="58"/>
-      <c r="R8" s="59"/>
-    </row>
-    <row r="9" spans="2:18" s="71" customFormat="1" ht="28.5" customHeight="1" thickBot="1">
-      <c r="B9" s="60" t="s">
+      <c r="J8" s="49"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="50"/>
+      <c r="O8" s="50"/>
+      <c r="P8" s="50"/>
+      <c r="Q8" s="50"/>
+      <c r="R8" s="51"/>
+    </row>
+    <row r="9" spans="2:18" s="63" customFormat="1" ht="28.5" customHeight="1" thickBot="1">
+      <c r="B9" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="61" t="s">
+      <c r="C9" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="D9" s="62" t="s">
+      <c r="D9" s="54" t="s">
         <v>70</v>
       </c>
-      <c r="E9" s="63" t="s">
+      <c r="E9" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="F9" s="65" t="s">
+      <c r="F9" s="57" t="s">
         <v>72</v>
       </c>
-      <c r="G9" s="64" t="s">
+      <c r="G9" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="H9" s="67" t="s">
+      <c r="H9" s="59" t="s">
         <v>74</v>
       </c>
-      <c r="I9" s="68" t="s">
+      <c r="I9" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="J9" s="69" t="s">
+      <c r="J9" s="61" t="s">
         <v>76</v>
       </c>
-      <c r="K9" s="64" t="s">
+      <c r="K9" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="L9" s="64" t="s">
+      <c r="L9" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="M9" s="64" t="s">
+      <c r="M9" s="56" t="s">
         <v>79</v>
       </c>
-      <c r="N9" s="64" t="s">
+      <c r="N9" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="O9" s="64" t="s">
+      <c r="O9" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="P9" s="64" t="s">
+      <c r="P9" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="Q9" s="64" t="s">
+      <c r="Q9" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="R9" s="70" t="s">
+      <c r="R9" s="62" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="10" spans="2:18" ht="53.25" customHeight="1">
-      <c r="B10" s="190" t="s">
+      <c r="B10" s="182" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="177" t="s">
+      <c r="C10" s="169" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="191" t="s">
+      <c r="D10" s="183" t="s">
         <v>85</v>
       </c>
-      <c r="E10" s="178" t="s">
+      <c r="E10" s="170" t="s">
         <v>86</v>
       </c>
-      <c r="F10" s="176" t="s">
+      <c r="F10" s="168" t="s">
         <v>87</v>
       </c>
-      <c r="G10" s="179" t="s">
+      <c r="G10" s="171" t="s">
         <v>88</v>
       </c>
-      <c r="H10" s="172" t="s">
+      <c r="H10" s="164" t="s">
         <v>89</v>
       </c>
-      <c r="I10" s="189" t="s">
+      <c r="I10" s="181" t="s">
         <v>90</v>
       </c>
-      <c r="J10" s="72" t="s">
+      <c r="J10" s="64" t="s">
         <v>91</v>
       </c>
-      <c r="K10" s="72" t="s">
+      <c r="K10" s="64" t="s">
         <v>92</v>
       </c>
-      <c r="L10" s="72"/>
-      <c r="M10" s="72"/>
-      <c r="N10" s="73"/>
-      <c r="O10" s="74" t="s">
+      <c r="L10" s="64"/>
+      <c r="M10" s="64"/>
+      <c r="N10" s="65"/>
+      <c r="O10" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="P10" s="73" t="s">
+      <c r="P10" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="Q10" s="73" t="s">
+      <c r="Q10" s="65" t="s">
         <v>94</v>
       </c>
-      <c r="R10" s="75"/>
+      <c r="R10" s="67"/>
     </row>
     <row r="11" spans="2:18" ht="45.75" customHeight="1">
-      <c r="B11" s="183" t="s">
+      <c r="B11" s="175" t="s">
         <v>95</v>
       </c>
-      <c r="C11" s="173" t="s">
+      <c r="C11" s="165" t="s">
         <v>96</v>
       </c>
-      <c r="D11" s="184" t="s">
+      <c r="D11" s="176" t="s">
         <v>97</v>
       </c>
-      <c r="E11" s="185" t="s">
+      <c r="E11" s="177" t="s">
         <v>98</v>
       </c>
-      <c r="F11" s="171" t="s">
+      <c r="F11" s="163" t="s">
         <v>99</v>
       </c>
-      <c r="G11" s="175" t="s">
+      <c r="G11" s="167" t="s">
         <v>100</v>
       </c>
-      <c r="H11" s="170" t="s">
+      <c r="H11" s="162" t="s">
         <v>89</v>
       </c>
-      <c r="I11" s="189" t="s">
+      <c r="I11" s="181" t="s">
         <v>90</v>
       </c>
-      <c r="J11" s="72" t="s">
+      <c r="J11" s="64" t="s">
         <v>91</v>
       </c>
-      <c r="K11" s="72" t="s">
+      <c r="K11" s="64" t="s">
         <v>92</v>
       </c>
-      <c r="L11" s="72"/>
-      <c r="M11" s="72"/>
-      <c r="N11" s="73">
+      <c r="L11" s="64"/>
+      <c r="M11" s="64"/>
+      <c r="N11" s="65">
         <v>50</v>
       </c>
-      <c r="O11" s="74" t="s">
+      <c r="O11" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="P11" s="73" t="s">
+      <c r="P11" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="Q11" s="73" t="s">
+      <c r="Q11" s="65" t="s">
         <v>101</v>
       </c>
-      <c r="R11" s="75"/>
+      <c r="R11" s="67"/>
     </row>
     <row r="12" spans="2:18" ht="43.5" customHeight="1">
-      <c r="B12" s="183" t="s">
+      <c r="B12" s="175" t="s">
         <v>102</v>
       </c>
-      <c r="C12" s="173" t="s">
+      <c r="C12" s="165" t="s">
         <v>103</v>
       </c>
-      <c r="D12" s="77" t="s">
+      <c r="D12" s="69" t="s">
         <v>104</v>
       </c>
-      <c r="E12" s="174" t="s">
+      <c r="E12" s="166" t="s">
         <v>86</v>
       </c>
-      <c r="F12" s="187" t="s">
+      <c r="F12" s="179" t="s">
         <v>105</v>
       </c>
-      <c r="G12" s="50" t="s">
+      <c r="G12" s="42" t="s">
         <v>88</v>
       </c>
-      <c r="H12" s="78" t="s">
+      <c r="H12" s="70" t="s">
         <v>89</v>
       </c>
-      <c r="I12" s="189" t="s">
+      <c r="I12" s="181" t="s">
         <v>90</v>
       </c>
-      <c r="J12" s="72" t="s">
+      <c r="J12" s="64" t="s">
         <v>91</v>
       </c>
-      <c r="K12" s="72" t="s">
+      <c r="K12" s="64" t="s">
         <v>92</v>
       </c>
-      <c r="L12" s="72"/>
-      <c r="M12" s="72"/>
-      <c r="N12" s="73">
+      <c r="L12" s="64"/>
+      <c r="M12" s="64"/>
+      <c r="N12" s="65">
         <v>50</v>
       </c>
-      <c r="O12" s="74" t="s">
+      <c r="O12" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="P12" s="73" t="s">
+      <c r="P12" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="Q12" s="73" t="s">
+      <c r="Q12" s="65" t="s">
         <v>101</v>
       </c>
-      <c r="R12" s="75"/>
+      <c r="R12" s="67"/>
     </row>
     <row r="13" spans="2:18" ht="70.5" customHeight="1">
-      <c r="B13" s="183" t="s">
+      <c r="B13" s="175" t="s">
         <v>106</v>
       </c>
-      <c r="C13" s="173" t="s">
+      <c r="C13" s="165" t="s">
         <v>107</v>
       </c>
-      <c r="D13" s="77" t="s">
+      <c r="D13" s="69" t="s">
         <v>108</v>
       </c>
-      <c r="E13" s="174" t="s">
+      <c r="E13" s="166" t="s">
         <v>98</v>
       </c>
-      <c r="F13" s="187" t="s">
+      <c r="F13" s="179" t="s">
         <v>105</v>
       </c>
-      <c r="G13" s="50" t="s">
+      <c r="G13" s="42" t="s">
         <v>100</v>
       </c>
-      <c r="H13" s="78" t="s">
+      <c r="H13" s="70" t="s">
         <v>89</v>
       </c>
-      <c r="I13" s="189" t="s">
+      <c r="I13" s="181" t="s">
         <v>90</v>
       </c>
-      <c r="J13" s="72" t="s">
+      <c r="J13" s="64" t="s">
         <v>91</v>
       </c>
-      <c r="K13" s="72" t="s">
+      <c r="K13" s="64" t="s">
         <v>92</v>
       </c>
-      <c r="L13" s="72"/>
-      <c r="M13" s="72"/>
-      <c r="N13" s="73"/>
-      <c r="O13" s="74" t="s">
+      <c r="L13" s="64"/>
+      <c r="M13" s="64"/>
+      <c r="N13" s="65"/>
+      <c r="O13" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="P13" s="73" t="s">
+      <c r="P13" s="65" t="s">
         <v>109</v>
       </c>
-      <c r="Q13" s="73" t="s">
+      <c r="Q13" s="65" t="s">
         <v>110</v>
       </c>
-      <c r="R13" s="75"/>
+      <c r="R13" s="67"/>
     </row>
     <row r="14" spans="2:18" ht="36.75" customHeight="1">
-      <c r="B14" s="183" t="s">
+      <c r="B14" s="175" t="s">
         <v>111</v>
       </c>
-      <c r="C14" s="173" t="s">
+      <c r="C14" s="165" t="s">
         <v>112</v>
       </c>
-      <c r="D14" s="77" t="s">
+      <c r="D14" s="69" t="s">
         <v>113</v>
       </c>
-      <c r="E14" s="174" t="s">
+      <c r="E14" s="166" t="s">
         <v>86</v>
       </c>
-      <c r="F14" s="188" t="s">
+      <c r="F14" s="180" t="s">
         <v>99</v>
       </c>
-      <c r="G14" s="50" t="s">
+      <c r="G14" s="42" t="s">
         <v>88</v>
       </c>
-      <c r="H14" s="78" t="s">
+      <c r="H14" s="70" t="s">
         <v>89</v>
       </c>
-      <c r="I14" s="189" t="s">
+      <c r="I14" s="181" t="s">
         <v>90</v>
       </c>
-      <c r="J14" s="72" t="s">
+      <c r="J14" s="64" t="s">
         <v>91</v>
       </c>
-      <c r="K14" s="72" t="s">
+      <c r="K14" s="64" t="s">
         <v>92</v>
       </c>
-      <c r="L14" s="72"/>
-      <c r="M14" s="72"/>
-      <c r="N14" s="73">
+      <c r="L14" s="64"/>
+      <c r="M14" s="64"/>
+      <c r="N14" s="65">
         <v>10</v>
       </c>
-      <c r="O14" s="74" t="s">
+      <c r="O14" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="P14" s="73" t="s">
+      <c r="P14" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="Q14" s="73" t="s">
+      <c r="Q14" s="65" t="s">
         <v>101</v>
       </c>
-      <c r="R14" s="75"/>
+      <c r="R14" s="67"/>
     </row>
     <row r="15" spans="2:18" ht="31.5" customHeight="1">
-      <c r="B15" s="137"/>
-      <c r="C15" s="173"/>
-      <c r="D15" s="77"/>
-      <c r="E15" s="186"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="50"/>
+      <c r="B15" s="129"/>
+      <c r="C15" s="165"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="178"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="42"/>
     </row>
     <row r="16" spans="2:18">
-      <c r="B16" s="137"/>
-      <c r="C16" s="173"/>
-      <c r="D16" s="77"/>
-      <c r="E16" s="186"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="50"/>
+      <c r="B16" s="129"/>
+      <c r="C16" s="165"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="178"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="42"/>
     </row>
     <row r="17" spans="1:19">
-      <c r="B17" s="137"/>
-      <c r="C17" s="173"/>
-      <c r="D17" s="77"/>
-      <c r="E17" s="186"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="50"/>
+      <c r="B17" s="129"/>
+      <c r="C17" s="165"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="178"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="42"/>
     </row>
     <row r="18" spans="1:19" ht="41.25" customHeight="1"/>
     <row r="19" spans="1:19" ht="6" customHeight="1">
-      <c r="A19" s="79"/>
-      <c r="B19" s="79"/>
-      <c r="C19" s="80"/>
-      <c r="D19" s="79"/>
-      <c r="E19" s="79"/>
-      <c r="F19" s="81"/>
-      <c r="G19" s="79"/>
-      <c r="H19" s="79"/>
-      <c r="I19" s="82"/>
-      <c r="J19" s="80"/>
-      <c r="K19" s="79"/>
-      <c r="L19" s="79"/>
-      <c r="M19" s="80"/>
-      <c r="N19" s="79"/>
-      <c r="O19" s="80"/>
-      <c r="P19" s="79"/>
-      <c r="Q19" s="79"/>
-      <c r="R19" s="79"/>
-      <c r="S19" s="79"/>
+      <c r="A19" s="71"/>
+      <c r="B19" s="71"/>
+      <c r="C19" s="72"/>
+      <c r="D19" s="71"/>
+      <c r="E19" s="71"/>
+      <c r="F19" s="73"/>
+      <c r="G19" s="71"/>
+      <c r="H19" s="71"/>
+      <c r="I19" s="74"/>
+      <c r="J19" s="72"/>
+      <c r="K19" s="71"/>
+      <c r="L19" s="71"/>
+      <c r="M19" s="72"/>
+      <c r="N19" s="71"/>
+      <c r="O19" s="72"/>
+      <c r="P19" s="71"/>
+      <c r="Q19" s="71"/>
+      <c r="R19" s="71"/>
+      <c r="S19" s="71"/>
     </row>
     <row r="20" spans="1:19" ht="14.1" hidden="1" customHeight="1"/>
     <row r="21" spans="1:19" ht="15" hidden="1" customHeight="1"/>
@@ -6383,396 +6672,396 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AG243"/>
   <sheetViews>
-    <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="B15" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.25" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.25" zeroHeight="1"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" style="24" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.42578125" style="24" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="41.5703125" style="24" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="42.42578125" style="83" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="14.140625" style="24" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="15.140625" style="24" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.85546875" style="24" customWidth="1" collapsed="1"/>
-    <col min="10" max="11" width="15.140625" style="84" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" style="49" customWidth="1" collapsed="1"/>
-    <col min="13" max="15" width="15.140625" style="24" customWidth="1" collapsed="1"/>
-    <col min="16" max="17" width="11.42578125" style="24" customWidth="1" collapsed="1"/>
-    <col min="18" max="23" width="11.42578125" style="24" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="11.42578125" style="24" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="11.42578125" style="24" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="33" width="11.42578125" style="24" hidden="1" customWidth="1"/>
-    <col min="34" max="16384" width="11.42578125" style="24" hidden="1" collapsed="1"/>
+    <col min="1" max="1" width="6.28515625" style="21" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.42578125" style="21" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="41.5703125" style="21" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="42.42578125" style="75" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="14.140625" style="21" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="15.140625" style="21" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.85546875" style="21" customWidth="1" collapsed="1"/>
+    <col min="10" max="11" width="15.140625" style="76" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" style="41" customWidth="1" collapsed="1"/>
+    <col min="13" max="15" width="15.140625" style="21" customWidth="1" collapsed="1"/>
+    <col min="16" max="17" width="11.42578125" style="21" customWidth="1" collapsed="1"/>
+    <col min="18" max="23" width="11.42578125" style="21" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="11.42578125" style="21" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="11.42578125" style="21" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="33" width="11.42578125" style="21" hidden="1" customWidth="1"/>
+    <col min="34" max="16384" width="11.42578125" style="21" hidden="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17"/>
     <row r="2" spans="1:17"/>
-    <row r="3" spans="1:17" s="85" customFormat="1">
-      <c r="D3" s="86"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="88"/>
-    </row>
-    <row r="4" spans="1:17" s="85" customFormat="1">
-      <c r="D4" s="86"/>
-      <c r="J4" s="87"/>
-      <c r="K4" s="87"/>
-      <c r="L4" s="88"/>
+    <row r="3" spans="1:17" s="77" customFormat="1">
+      <c r="D3" s="78"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
+      <c r="L3" s="80"/>
+    </row>
+    <row r="4" spans="1:17" s="77" customFormat="1">
+      <c r="D4" s="78"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="79"/>
+      <c r="L4" s="80"/>
     </row>
     <row r="5" spans="1:17"/>
     <row r="6" spans="1:17"/>
     <row r="7" spans="1:17" ht="23.25">
-      <c r="C7" s="90" t="s">
+      <c r="C7" s="82" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="92" customFormat="1" ht="44.1" customHeight="1">
-      <c r="A8" s="89"/>
-      <c r="B8" s="89"/>
-      <c r="D8" s="240" t="s">
+    <row r="8" spans="1:17" s="84" customFormat="1" ht="44.1" customHeight="1">
+      <c r="A8" s="81"/>
+      <c r="B8" s="81"/>
+      <c r="D8" s="229" t="s">
         <v>176</v>
       </c>
-      <c r="E8" s="91"/>
-      <c r="H8" s="93"/>
-      <c r="I8" s="91"/>
-      <c r="J8" s="93"/>
-      <c r="K8" s="94"/>
-      <c r="L8" s="95"/>
-      <c r="M8" s="89"/>
-      <c r="N8" s="89"/>
-      <c r="O8" s="89"/>
-      <c r="P8" s="89"/>
-      <c r="Q8" s="89"/>
+      <c r="E8" s="83"/>
+      <c r="H8" s="85"/>
+      <c r="I8" s="83"/>
+      <c r="J8" s="85"/>
+      <c r="K8" s="86"/>
+      <c r="L8" s="87"/>
+      <c r="M8" s="81"/>
+      <c r="N8" s="81"/>
+      <c r="O8" s="81"/>
+      <c r="P8" s="81"/>
+      <c r="Q8" s="81"/>
     </row>
     <row r="9" spans="1:17" ht="28.5" customHeight="1">
-      <c r="D9" s="24"/>
-      <c r="F9" s="83"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="96"/>
+      <c r="D9" s="21"/>
+      <c r="F9" s="75"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="88"/>
     </row>
     <row r="10" spans="1:17" ht="15" thickBot="1">
-      <c r="I10" s="97"/>
-    </row>
-    <row r="11" spans="1:17" s="99" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A11" s="98"/>
-      <c r="B11" s="224" t="s">
+      <c r="I10" s="89"/>
+    </row>
+    <row r="11" spans="1:17" s="91" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
+      <c r="A11" s="90"/>
+      <c r="B11" s="213" t="s">
         <v>114</v>
       </c>
-      <c r="C11" s="225"/>
-      <c r="D11" s="226" t="s">
+      <c r="C11" s="214"/>
+      <c r="D11" s="215" t="s">
         <v>115</v>
       </c>
-      <c r="E11" s="225"/>
-      <c r="F11" s="225"/>
-      <c r="G11" s="238" t="s">
+      <c r="E11" s="214"/>
+      <c r="F11" s="214"/>
+      <c r="G11" s="227" t="s">
         <v>116</v>
       </c>
-      <c r="H11" s="227"/>
-      <c r="I11" s="227"/>
-      <c r="J11" s="227"/>
-      <c r="K11" s="227"/>
-      <c r="L11" s="228"/>
-      <c r="M11" s="239" t="s">
+      <c r="H11" s="216"/>
+      <c r="I11" s="216"/>
+      <c r="J11" s="216"/>
+      <c r="K11" s="216"/>
+      <c r="L11" s="217"/>
+      <c r="M11" s="228" t="s">
         <v>117</v>
       </c>
-      <c r="N11" s="229"/>
-      <c r="O11" s="230"/>
+      <c r="N11" s="218"/>
+      <c r="O11" s="219"/>
     </row>
     <row r="12" spans="1:17" ht="26.25" thickBot="1">
-      <c r="B12" s="100" t="s">
+      <c r="B12" s="92" t="s">
         <v>118</v>
       </c>
-      <c r="C12" s="101" t="s">
+      <c r="C12" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="100" t="s">
+      <c r="D12" s="92" t="s">
         <v>119</v>
       </c>
-      <c r="E12" s="101" t="s">
+      <c r="E12" s="93" t="s">
         <v>120</v>
       </c>
-      <c r="F12" s="102" t="s">
+      <c r="F12" s="94" t="s">
         <v>121</v>
       </c>
-      <c r="G12" s="102" t="s">
+      <c r="G12" s="94" t="s">
         <v>122</v>
       </c>
-      <c r="H12" s="102" t="s">
+      <c r="H12" s="94" t="s">
         <v>123</v>
       </c>
-      <c r="I12" s="101" t="s">
+      <c r="I12" s="93" t="s">
         <v>124</v>
       </c>
-      <c r="J12" s="103" t="s">
+      <c r="J12" s="95" t="s">
         <v>125</v>
       </c>
-      <c r="K12" s="103" t="s">
+      <c r="K12" s="95" t="s">
         <v>126</v>
       </c>
-      <c r="L12" s="102" t="s">
+      <c r="L12" s="94" t="s">
         <v>127</v>
       </c>
-      <c r="M12" s="100" t="s">
+      <c r="M12" s="92" t="s">
         <v>128</v>
       </c>
-      <c r="N12" s="101" t="s">
+      <c r="N12" s="93" t="s">
         <v>129</v>
       </c>
-      <c r="O12" s="104" t="s">
+      <c r="O12" s="96" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="77.25" customHeight="1">
-      <c r="B13" s="246" t="s">
+      <c r="B13" s="235" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="245" t="s">
+      <c r="C13" s="234" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="107" t="s">
+      <c r="D13" s="99" t="s">
         <v>131</v>
       </c>
-      <c r="E13" s="105" t="s">
+      <c r="E13" s="97" t="s">
         <v>132</v>
       </c>
-      <c r="F13" s="106" t="s">
+      <c r="F13" s="98" t="s">
         <v>133</v>
       </c>
-      <c r="G13" s="199"/>
-      <c r="H13" s="200"/>
-      <c r="I13" s="108">
+      <c r="G13" s="191"/>
+      <c r="H13" s="192"/>
+      <c r="I13" s="100">
         <v>1</v>
       </c>
-      <c r="J13" s="108">
+      <c r="J13" s="100">
         <v>1</v>
       </c>
-      <c r="K13" s="203"/>
-      <c r="L13" s="109" t="e">
+      <c r="K13" s="195"/>
+      <c r="L13" s="101" t="e">
         <v>#REF!</v>
       </c>
-      <c r="M13" s="110">
+      <c r="M13" s="102">
         <v>45769</v>
       </c>
-      <c r="N13" s="111"/>
-      <c r="O13" s="112"/>
+      <c r="N13" s="103"/>
+      <c r="O13" s="104"/>
     </row>
     <row r="14" spans="1:17" ht="77.25" customHeight="1">
-      <c r="B14" s="247"/>
-      <c r="C14" s="248"/>
-      <c r="D14" s="115" t="s">
+      <c r="B14" s="236"/>
+      <c r="C14" s="237"/>
+      <c r="D14" s="107" t="s">
         <v>134</v>
       </c>
-      <c r="E14" s="105" t="s">
+      <c r="E14" s="97" t="s">
         <v>132</v>
       </c>
-      <c r="F14" s="114" t="s">
+      <c r="F14" s="106" t="s">
         <v>135</v>
       </c>
-      <c r="G14" s="199"/>
-      <c r="H14" s="200"/>
-      <c r="I14" s="108">
+      <c r="G14" s="191"/>
+      <c r="H14" s="192"/>
+      <c r="I14" s="100">
         <v>1</v>
       </c>
-      <c r="J14" s="108">
+      <c r="J14" s="100">
         <v>1</v>
       </c>
-      <c r="K14" s="203"/>
-      <c r="L14" s="109" t="e">
+      <c r="K14" s="195"/>
+      <c r="L14" s="101" t="e">
         <v>#REF!</v>
       </c>
-      <c r="M14" s="110">
+      <c r="M14" s="102">
         <v>45769</v>
       </c>
-      <c r="N14" s="116"/>
-      <c r="O14" s="117"/>
+      <c r="N14" s="108"/>
+      <c r="O14" s="109"/>
     </row>
     <row r="15" spans="1:17" ht="77.25" customHeight="1">
-      <c r="B15" s="246" t="s">
+      <c r="B15" s="235" t="s">
         <v>106</v>
       </c>
-      <c r="C15" s="245" t="s">
+      <c r="C15" s="234" t="s">
         <v>136</v>
       </c>
-      <c r="D15" s="115" t="s">
+      <c r="D15" s="107" t="s">
         <v>137</v>
       </c>
-      <c r="E15" s="113" t="s">
+      <c r="E15" s="105" t="s">
         <v>138</v>
       </c>
-      <c r="F15" s="114" t="s">
+      <c r="F15" s="106" t="s">
         <v>133</v>
       </c>
-      <c r="G15" s="199"/>
-      <c r="H15" s="200"/>
-      <c r="I15" s="108">
+      <c r="G15" s="191"/>
+      <c r="H15" s="192"/>
+      <c r="I15" s="100">
         <v>0.7</v>
       </c>
-      <c r="J15" s="108"/>
-      <c r="K15" s="203"/>
-      <c r="L15" s="109" t="e">
+      <c r="J15" s="100"/>
+      <c r="K15" s="195"/>
+      <c r="L15" s="101" t="e">
         <v>#REF!</v>
       </c>
-      <c r="M15" s="110">
+      <c r="M15" s="102">
         <v>45769</v>
       </c>
-      <c r="N15" s="116"/>
-      <c r="O15" s="117"/>
+      <c r="N15" s="108"/>
+      <c r="O15" s="109"/>
     </row>
     <row r="16" spans="1:17" ht="77.25" customHeight="1">
-      <c r="B16" s="247"/>
-      <c r="C16" s="248"/>
-      <c r="D16" s="115" t="s">
+      <c r="B16" s="236"/>
+      <c r="C16" s="237"/>
+      <c r="D16" s="107" t="s">
         <v>139</v>
       </c>
-      <c r="E16" s="113" t="s">
+      <c r="E16" s="105" t="s">
         <v>138</v>
       </c>
-      <c r="F16" s="114" t="s">
+      <c r="F16" s="106" t="s">
         <v>135</v>
       </c>
-      <c r="G16" s="199"/>
-      <c r="H16" s="200"/>
-      <c r="I16" s="108">
+      <c r="G16" s="191"/>
+      <c r="H16" s="192"/>
+      <c r="I16" s="100">
         <v>0.8</v>
       </c>
-      <c r="J16" s="108"/>
-      <c r="K16" s="203"/>
-      <c r="L16" s="109" t="e">
+      <c r="J16" s="100"/>
+      <c r="K16" s="195"/>
+      <c r="L16" s="101" t="e">
         <v>#REF!</v>
       </c>
-      <c r="M16" s="110">
+      <c r="M16" s="102">
         <v>45769</v>
       </c>
-      <c r="N16" s="116"/>
-      <c r="O16" s="117"/>
+      <c r="N16" s="108"/>
+      <c r="O16" s="109"/>
     </row>
     <row r="17" spans="2:23" ht="77.25" customHeight="1">
-      <c r="B17" s="246" t="s">
+      <c r="B17" s="235" t="s">
         <v>111</v>
       </c>
-      <c r="C17" s="244" t="s">
+      <c r="C17" s="233" t="s">
         <v>112</v>
       </c>
-      <c r="D17" s="115" t="s">
+      <c r="D17" s="107" t="s">
         <v>140</v>
       </c>
-      <c r="E17" s="113" t="s">
+      <c r="E17" s="105" t="s">
         <v>132</v>
       </c>
-      <c r="F17" s="114" t="s">
+      <c r="F17" s="106" t="s">
         <v>133</v>
       </c>
-      <c r="G17" s="199"/>
-      <c r="H17" s="200"/>
-      <c r="I17" s="108">
+      <c r="G17" s="191"/>
+      <c r="H17" s="192"/>
+      <c r="I17" s="100">
         <v>0.7</v>
       </c>
-      <c r="J17" s="108"/>
-      <c r="K17" s="203"/>
-      <c r="L17" s="109"/>
-      <c r="M17" s="110">
+      <c r="J17" s="100"/>
+      <c r="K17" s="195"/>
+      <c r="L17" s="101"/>
+      <c r="M17" s="102">
         <v>45769</v>
       </c>
-      <c r="N17" s="116"/>
-      <c r="O17" s="117"/>
+      <c r="N17" s="108"/>
+      <c r="O17" s="109"/>
     </row>
     <row r="18" spans="2:23" ht="77.25" customHeight="1">
-      <c r="B18" s="247"/>
-      <c r="C18" s="245"/>
-      <c r="D18" s="115" t="s">
+      <c r="B18" s="236"/>
+      <c r="C18" s="234"/>
+      <c r="D18" s="107" t="s">
         <v>141</v>
       </c>
-      <c r="E18" s="113" t="s">
+      <c r="E18" s="105" t="s">
         <v>132</v>
       </c>
-      <c r="F18" s="114" t="s">
+      <c r="F18" s="106" t="s">
         <v>135</v>
       </c>
-      <c r="G18" s="199"/>
-      <c r="H18" s="200"/>
-      <c r="I18" s="108">
+      <c r="G18" s="191"/>
+      <c r="H18" s="192"/>
+      <c r="I18" s="100">
         <v>0.6</v>
       </c>
-      <c r="J18" s="108"/>
-      <c r="K18" s="203"/>
-      <c r="L18" s="109"/>
-      <c r="M18" s="110">
+      <c r="J18" s="100"/>
+      <c r="K18" s="195"/>
+      <c r="L18" s="101"/>
+      <c r="M18" s="102">
         <v>45769</v>
       </c>
-      <c r="N18" s="116"/>
-      <c r="O18" s="117"/>
+      <c r="N18" s="108"/>
+      <c r="O18" s="109"/>
     </row>
     <row r="19" spans="2:23" ht="77.25" customHeight="1">
-      <c r="B19" s="180"/>
-      <c r="C19" s="181"/>
-      <c r="D19" s="115"/>
-      <c r="E19" s="113"/>
-      <c r="F19" s="114"/>
-      <c r="G19" s="199"/>
-      <c r="H19" s="200"/>
-      <c r="I19" s="108"/>
-      <c r="J19" s="108"/>
-      <c r="K19" s="203"/>
-      <c r="L19" s="109"/>
-      <c r="M19" s="110"/>
-      <c r="N19" s="116"/>
-      <c r="O19" s="117"/>
+      <c r="B19" s="172"/>
+      <c r="C19" s="173"/>
+      <c r="D19" s="107"/>
+      <c r="E19" s="105"/>
+      <c r="F19" s="106"/>
+      <c r="G19" s="191"/>
+      <c r="H19" s="192"/>
+      <c r="I19" s="100"/>
+      <c r="J19" s="100"/>
+      <c r="K19" s="195"/>
+      <c r="L19" s="101"/>
+      <c r="M19" s="102"/>
+      <c r="N19" s="108"/>
+      <c r="O19" s="109"/>
     </row>
     <row r="20" spans="2:23" ht="77.25" customHeight="1">
-      <c r="B20" s="180"/>
-      <c r="C20" s="181"/>
-      <c r="D20" s="115"/>
-      <c r="E20" s="113"/>
-      <c r="F20" s="114"/>
-      <c r="G20" s="199"/>
-      <c r="H20" s="200"/>
-      <c r="I20" s="108"/>
-      <c r="J20" s="108"/>
-      <c r="K20" s="203"/>
-      <c r="L20" s="109"/>
-      <c r="M20" s="110"/>
-      <c r="N20" s="116"/>
-      <c r="O20" s="117"/>
+      <c r="B20" s="172"/>
+      <c r="C20" s="173"/>
+      <c r="D20" s="107"/>
+      <c r="E20" s="105"/>
+      <c r="F20" s="106"/>
+      <c r="G20" s="191"/>
+      <c r="H20" s="192"/>
+      <c r="I20" s="100"/>
+      <c r="J20" s="100"/>
+      <c r="K20" s="195"/>
+      <c r="L20" s="101"/>
+      <c r="M20" s="102"/>
+      <c r="N20" s="108"/>
+      <c r="O20" s="109"/>
     </row>
     <row r="21" spans="2:23">
-      <c r="B21" s="267"/>
-      <c r="C21" s="269"/>
-      <c r="D21" s="115"/>
-      <c r="E21" s="113"/>
-      <c r="F21" s="114"/>
-      <c r="G21" s="199"/>
-      <c r="H21" s="200"/>
-      <c r="I21" s="108"/>
-      <c r="J21" s="108"/>
-      <c r="K21" s="203"/>
-      <c r="L21" s="109"/>
-      <c r="M21" s="110"/>
-      <c r="N21" s="116"/>
-      <c r="O21" s="117"/>
+      <c r="B21" s="268"/>
+      <c r="C21" s="270"/>
+      <c r="D21" s="107"/>
+      <c r="E21" s="105"/>
+      <c r="F21" s="106"/>
+      <c r="G21" s="191"/>
+      <c r="H21" s="192"/>
+      <c r="I21" s="100"/>
+      <c r="J21" s="100"/>
+      <c r="K21" s="195"/>
+      <c r="L21" s="101"/>
+      <c r="M21" s="102"/>
+      <c r="N21" s="108"/>
+      <c r="O21" s="109"/>
     </row>
     <row r="22" spans="2:23" ht="15" thickBot="1">
-      <c r="B22" s="268"/>
-      <c r="C22" s="270"/>
-      <c r="D22" s="120"/>
-      <c r="E22" s="118"/>
-      <c r="F22" s="119"/>
-      <c r="G22" s="201"/>
-      <c r="H22" s="202"/>
-      <c r="I22" s="121"/>
-      <c r="J22" s="121"/>
-      <c r="K22" s="204"/>
-      <c r="L22" s="122"/>
-      <c r="M22" s="123"/>
-      <c r="N22" s="124"/>
-      <c r="O22" s="125"/>
+      <c r="B22" s="269"/>
+      <c r="C22" s="271"/>
+      <c r="D22" s="112"/>
+      <c r="E22" s="110"/>
+      <c r="F22" s="111"/>
+      <c r="G22" s="193"/>
+      <c r="H22" s="194"/>
+      <c r="I22" s="113"/>
+      <c r="J22" s="113"/>
+      <c r="K22" s="196"/>
+      <c r="L22" s="114"/>
+      <c r="M22" s="115"/>
+      <c r="N22" s="116"/>
+      <c r="O22" s="117"/>
     </row>
     <row r="23" spans="2:23">
-      <c r="D23" s="24"/>
-      <c r="J23" s="24"/>
-      <c r="K23" s="24"/>
-      <c r="L23" s="24"/>
+      <c r="D23" s="21"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="21"/>
     </row>
     <row r="24" spans="2:23"/>
     <row r="25" spans="2:23"/>
@@ -6780,7 +7069,7 @@
     <row r="27" spans="2:23"/>
     <row r="28" spans="2:23"/>
     <row r="29" spans="2:23" s="16" customFormat="1" ht="3.75" customHeight="1">
-      <c r="W29" s="126"/>
+      <c r="W29" s="118"/>
     </row>
     <row r="30" spans="2:23"/>
     <row r="31" spans="2:23" ht="14.25" customHeight="1"/>
@@ -6956,7 +7245,8 @@
     <mergeCell ref="C21:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6968,42 +7258,42 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col min="1" max="1" width="1.85546875" style="99" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="99" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" style="127" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" style="99" customWidth="1"/>
-    <col min="5" max="5" width="34.140625" style="99" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.140625" style="99" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="36.140625" style="99" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" style="99" customWidth="1"/>
-    <col min="10" max="10" width="29" style="99" customWidth="1"/>
-    <col min="11" max="11" width="21.42578125" style="99" customWidth="1"/>
-    <col min="12" max="12" width="13" style="99" customWidth="1"/>
-    <col min="13" max="13" width="18" style="128" customWidth="1"/>
-    <col min="14" max="14" width="27.5703125" style="99" customWidth="1"/>
-    <col min="15" max="15" width="40.42578125" style="99" customWidth="1"/>
-    <col min="16" max="17" width="15.140625" style="99" customWidth="1"/>
-    <col min="18" max="18" width="21.42578125" style="99" customWidth="1"/>
-    <col min="19" max="20" width="28.5703125" style="129" customWidth="1"/>
-    <col min="21" max="21" width="20.85546875" style="99" customWidth="1"/>
-    <col min="22" max="22" width="10.42578125" style="99" customWidth="1"/>
-    <col min="23" max="23" width="14.140625" style="99" hidden="1" customWidth="1"/>
-    <col min="24" max="39" width="11.5703125" style="99" hidden="1" customWidth="1"/>
-    <col min="40" max="16384" width="11.42578125" style="99" hidden="1"/>
+    <col min="1" max="1" width="1.85546875" style="91" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="91" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" style="119" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" style="91" customWidth="1"/>
+    <col min="5" max="5" width="34.140625" style="91" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.140625" style="91" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="36.140625" style="91" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" style="91" customWidth="1"/>
+    <col min="10" max="10" width="29" style="91" customWidth="1"/>
+    <col min="11" max="11" width="21.42578125" style="91" customWidth="1"/>
+    <col min="12" max="12" width="13" style="91" customWidth="1"/>
+    <col min="13" max="13" width="18" style="120" customWidth="1"/>
+    <col min="14" max="14" width="27.5703125" style="91" customWidth="1"/>
+    <col min="15" max="15" width="40.42578125" style="91" customWidth="1"/>
+    <col min="16" max="17" width="15.140625" style="91" customWidth="1"/>
+    <col min="18" max="18" width="21.42578125" style="91" customWidth="1"/>
+    <col min="19" max="20" width="28.5703125" style="121" customWidth="1"/>
+    <col min="21" max="21" width="20.85546875" style="91" customWidth="1"/>
+    <col min="22" max="22" width="10.42578125" style="91" customWidth="1"/>
+    <col min="23" max="23" width="14.140625" style="91" hidden="1" customWidth="1"/>
+    <col min="24" max="39" width="11.5703125" style="91" hidden="1" customWidth="1"/>
+    <col min="40" max="16384" width="11.42578125" style="91" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" ht="14.25"/>
     <row r="2" spans="1:38" ht="14.25">
-      <c r="J2" s="128"/>
-      <c r="M2" s="99"/>
-      <c r="N2" s="129"/>
-      <c r="S2" s="99"/>
-      <c r="T2" s="99"/>
-    </row>
-    <row r="3" spans="1:38" s="85" customFormat="1" ht="30" customHeight="1">
-      <c r="C3" s="130"/>
+      <c r="J2" s="120"/>
+      <c r="M2" s="91"/>
+      <c r="N2" s="121"/>
+      <c r="S2" s="91"/>
+      <c r="T2" s="91"/>
+    </row>
+    <row r="3" spans="1:38" s="77" customFormat="1" ht="30" customHeight="1">
+      <c r="C3" s="122"/>
       <c r="D3" s="2" t="s">
         <v>179</v>
       </c>
@@ -7014,294 +7304,294 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:38" s="85" customFormat="1" ht="22.5" customHeight="1">
-      <c r="C4" s="130"/>
-      <c r="D4" s="86" t="s">
+    <row r="4" spans="1:38" s="77" customFormat="1" ht="22.5" customHeight="1">
+      <c r="C4" s="122"/>
+      <c r="D4" s="78" t="s">
         <v>142</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="86"/>
+      <c r="I4" s="78"/>
     </row>
     <row r="5" spans="1:38" ht="14.25">
-      <c r="E5" s="86"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="86"/>
-      <c r="H5" s="86"/>
-      <c r="J5" s="128"/>
-      <c r="L5" s="128"/>
-      <c r="M5" s="99"/>
-      <c r="O5" s="129"/>
-      <c r="P5" s="129"/>
-      <c r="Q5" s="129"/>
-      <c r="R5" s="129"/>
-      <c r="S5" s="99"/>
-      <c r="T5" s="99"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="78"/>
+      <c r="J5" s="120"/>
+      <c r="L5" s="120"/>
+      <c r="M5" s="91"/>
+      <c r="O5" s="121"/>
+      <c r="P5" s="121"/>
+      <c r="Q5" s="121"/>
+      <c r="R5" s="121"/>
+      <c r="S5" s="91"/>
+      <c r="T5" s="91"/>
     </row>
     <row r="6" spans="1:38" ht="14.25">
-      <c r="L6" s="128"/>
-      <c r="M6" s="99"/>
-      <c r="O6" s="129"/>
-      <c r="P6" s="129"/>
-      <c r="Q6" s="129"/>
-      <c r="R6" s="129"/>
-      <c r="S6" s="99"/>
-      <c r="T6" s="99"/>
+      <c r="L6" s="120"/>
+      <c r="M6" s="91"/>
+      <c r="O6" s="121"/>
+      <c r="P6" s="121"/>
+      <c r="Q6" s="121"/>
+      <c r="R6" s="121"/>
+      <c r="S6" s="91"/>
+      <c r="T6" s="91"/>
     </row>
     <row r="7" spans="1:38" ht="14.25">
-      <c r="L7" s="128"/>
-      <c r="M7" s="99"/>
-      <c r="O7" s="129"/>
-      <c r="P7" s="129"/>
-      <c r="Q7" s="129"/>
-      <c r="R7" s="129"/>
-      <c r="S7" s="99"/>
-      <c r="T7" s="99"/>
+      <c r="L7" s="120"/>
+      <c r="M7" s="91"/>
+      <c r="O7" s="121"/>
+      <c r="P7" s="121"/>
+      <c r="Q7" s="121"/>
+      <c r="R7" s="121"/>
+      <c r="S7" s="91"/>
+      <c r="T7" s="91"/>
     </row>
     <row r="8" spans="1:38" ht="14.25"/>
     <row r="9" spans="1:38" ht="14.25"/>
     <row r="10" spans="1:38" ht="15" thickBot="1"/>
     <row r="11" spans="1:38" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B11" s="237" t="s">
+      <c r="B11" s="226" t="s">
         <v>143</v>
       </c>
-      <c r="C11" s="235"/>
-      <c r="D11" s="235"/>
-      <c r="E11" s="235"/>
-      <c r="F11" s="236"/>
-      <c r="G11" s="234" t="s">
+      <c r="C11" s="224"/>
+      <c r="D11" s="224"/>
+      <c r="E11" s="224"/>
+      <c r="F11" s="225"/>
+      <c r="G11" s="223" t="s">
         <v>144</v>
       </c>
-      <c r="H11" s="235"/>
-      <c r="I11" s="235"/>
-      <c r="J11" s="236"/>
-      <c r="K11" s="249" t="s">
+      <c r="H11" s="224"/>
+      <c r="I11" s="224"/>
+      <c r="J11" s="225"/>
+      <c r="K11" s="238" t="s">
         <v>145</v>
       </c>
-      <c r="L11" s="231"/>
-      <c r="M11" s="231"/>
-      <c r="N11" s="231"/>
-      <c r="O11" s="231"/>
-      <c r="P11" s="232"/>
-      <c r="Q11" s="232"/>
-      <c r="R11" s="232"/>
-      <c r="S11" s="233"/>
-      <c r="T11" s="131"/>
-      <c r="U11" s="132" t="s">
+      <c r="L11" s="220"/>
+      <c r="M11" s="220"/>
+      <c r="N11" s="220"/>
+      <c r="O11" s="220"/>
+      <c r="P11" s="221"/>
+      <c r="Q11" s="221"/>
+      <c r="R11" s="221"/>
+      <c r="S11" s="222"/>
+      <c r="T11" s="123"/>
+      <c r="U11" s="124" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:38" ht="45" customHeight="1" thickBot="1">
-      <c r="B12" s="133" t="s">
+      <c r="B12" s="125" t="s">
         <v>146</v>
       </c>
-      <c r="C12" s="64" t="s">
+      <c r="C12" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="64" t="s">
+      <c r="D12" s="56" t="s">
         <v>147</v>
       </c>
-      <c r="E12" s="64" t="s">
+      <c r="E12" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="F12" s="63" t="s">
+      <c r="F12" s="55" t="s">
         <v>148</v>
       </c>
-      <c r="G12" s="134" t="s">
+      <c r="G12" s="126" t="s">
         <v>149</v>
       </c>
-      <c r="H12" s="134" t="s">
+      <c r="H12" s="126" t="s">
         <v>150</v>
       </c>
-      <c r="I12" s="64" t="s">
+      <c r="I12" s="56" t="s">
         <v>151</v>
       </c>
-      <c r="J12" s="63" t="s">
+      <c r="J12" s="55" t="s">
         <v>152</v>
       </c>
-      <c r="K12" s="135" t="s">
+      <c r="K12" s="127" t="s">
         <v>153</v>
       </c>
-      <c r="L12" s="64" t="s">
+      <c r="L12" s="56" t="s">
         <v>154</v>
       </c>
-      <c r="M12" s="64" t="s">
+      <c r="M12" s="56" t="s">
         <v>155</v>
       </c>
-      <c r="N12" s="64" t="s">
+      <c r="N12" s="56" t="s">
         <v>156</v>
       </c>
-      <c r="O12" s="64" t="s">
+      <c r="O12" s="56" t="s">
         <v>157</v>
       </c>
-      <c r="P12" s="134" t="s">
+      <c r="P12" s="126" t="s">
         <v>158</v>
       </c>
-      <c r="Q12" s="134" t="s">
+      <c r="Q12" s="126" t="s">
         <v>159</v>
       </c>
-      <c r="R12" s="134" t="s">
+      <c r="R12" s="126" t="s">
         <v>160</v>
       </c>
-      <c r="S12" s="63" t="s">
+      <c r="S12" s="55" t="s">
         <v>161</v>
       </c>
-      <c r="T12" s="66" t="s">
+      <c r="T12" s="58" t="s">
         <v>162</v>
       </c>
-      <c r="U12" s="136" t="s">
+      <c r="U12" s="128" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="13" spans="1:38" s="127" customFormat="1" ht="261.75" customHeight="1">
-      <c r="A13" s="137"/>
-      <c r="B13" s="138" t="s">
+    <row r="13" spans="1:38" s="119" customFormat="1" ht="261.75" customHeight="1">
+      <c r="A13" s="129"/>
+      <c r="B13" s="130" t="s">
         <v>111</v>
       </c>
-      <c r="C13" s="139" t="s">
+      <c r="C13" s="131" t="s">
         <v>112</v>
       </c>
-      <c r="D13" s="140" t="s">
+      <c r="D13" s="132" t="s">
         <v>163</v>
       </c>
-      <c r="E13" s="141"/>
-      <c r="F13" s="142"/>
-      <c r="G13" s="143" t="s">
+      <c r="E13" s="133"/>
+      <c r="F13" s="134"/>
+      <c r="G13" s="135" t="s">
         <v>164</v>
       </c>
-      <c r="H13" s="143" t="s">
+      <c r="H13" s="135" t="s">
         <v>165</v>
       </c>
-      <c r="I13" s="73">
+      <c r="I13" s="65">
         <v>1</v>
       </c>
-      <c r="J13" s="144" t="s">
+      <c r="J13" s="136" t="s">
         <v>166</v>
       </c>
-      <c r="K13" s="145" t="s">
+      <c r="K13" s="137" t="s">
         <v>167</v>
       </c>
-      <c r="L13" s="146"/>
-      <c r="M13" s="146"/>
-      <c r="N13" s="147" t="s">
+      <c r="L13" s="138"/>
+      <c r="M13" s="138"/>
+      <c r="N13" s="139" t="s">
         <v>168</v>
       </c>
-      <c r="O13" s="147"/>
-      <c r="P13" s="148"/>
-      <c r="Q13" s="148"/>
-      <c r="R13" s="148" t="s">
+      <c r="O13" s="139"/>
+      <c r="P13" s="140"/>
+      <c r="Q13" s="140"/>
+      <c r="R13" s="140" t="s">
         <v>169</v>
       </c>
-      <c r="S13" s="149" t="s">
+      <c r="S13" s="141" t="s">
         <v>170</v>
       </c>
-      <c r="T13" s="150"/>
-      <c r="U13" s="151">
+      <c r="T13" s="142"/>
+      <c r="U13" s="143">
         <v>45748</v>
       </c>
-      <c r="V13" s="137"/>
-      <c r="W13" s="137"/>
-      <c r="X13" s="137"/>
-    </row>
-    <row r="14" spans="1:38" s="127" customFormat="1" ht="261.75" customHeight="1" thickBot="1">
-      <c r="A14" s="137"/>
-      <c r="B14" s="152"/>
-      <c r="C14" s="153"/>
-      <c r="D14" s="154"/>
-      <c r="E14" s="155"/>
-      <c r="F14" s="156"/>
-      <c r="G14" s="157"/>
-      <c r="H14" s="157"/>
-      <c r="I14" s="76">
+      <c r="V13" s="129"/>
+      <c r="W13" s="129"/>
+      <c r="X13" s="129"/>
+    </row>
+    <row r="14" spans="1:38" s="119" customFormat="1" ht="261.75" customHeight="1" thickBot="1">
+      <c r="A14" s="129"/>
+      <c r="B14" s="144"/>
+      <c r="C14" s="145"/>
+      <c r="D14" s="146"/>
+      <c r="E14" s="147"/>
+      <c r="F14" s="148"/>
+      <c r="G14" s="149"/>
+      <c r="H14" s="149"/>
+      <c r="I14" s="68">
         <v>1</v>
       </c>
-      <c r="J14" s="158"/>
-      <c r="K14" s="159"/>
-      <c r="L14" s="160"/>
-      <c r="M14" s="160"/>
-      <c r="N14" s="161"/>
-      <c r="O14" s="161"/>
-      <c r="P14" s="162"/>
-      <c r="Q14" s="162"/>
-      <c r="R14" s="162"/>
-      <c r="S14" s="163"/>
-      <c r="T14" s="164"/>
-      <c r="U14" s="165">
+      <c r="J14" s="150"/>
+      <c r="K14" s="151"/>
+      <c r="L14" s="152"/>
+      <c r="M14" s="152"/>
+      <c r="N14" s="153"/>
+      <c r="O14" s="153"/>
+      <c r="P14" s="154"/>
+      <c r="Q14" s="154"/>
+      <c r="R14" s="154"/>
+      <c r="S14" s="155"/>
+      <c r="T14" s="156"/>
+      <c r="U14" s="157">
         <v>45413</v>
       </c>
-      <c r="V14" s="35"/>
-      <c r="W14" s="35"/>
-      <c r="X14" s="35"/>
-      <c r="Y14" s="99"/>
-      <c r="Z14" s="99"/>
-      <c r="AA14" s="99"/>
-      <c r="AB14" s="99"/>
-      <c r="AC14" s="99"/>
-      <c r="AD14" s="99"/>
-      <c r="AE14" s="99"/>
-      <c r="AF14" s="99"/>
-      <c r="AG14" s="99"/>
-      <c r="AH14" s="99"/>
-      <c r="AI14" s="99"/>
-      <c r="AJ14" s="99"/>
-      <c r="AK14" s="99"/>
-      <c r="AL14" s="99"/>
-    </row>
-    <row r="15" spans="1:38" s="127" customFormat="1" ht="261.75" customHeight="1" thickBot="1">
-      <c r="A15" s="137"/>
-      <c r="B15" s="152"/>
-      <c r="C15" s="153"/>
-      <c r="D15" s="154"/>
-      <c r="E15" s="155"/>
-      <c r="F15" s="156"/>
-      <c r="G15" s="157"/>
-      <c r="H15" s="157"/>
-      <c r="I15" s="76">
+      <c r="V14" s="31"/>
+      <c r="W14" s="31"/>
+      <c r="X14" s="31"/>
+      <c r="Y14" s="91"/>
+      <c r="Z14" s="91"/>
+      <c r="AA14" s="91"/>
+      <c r="AB14" s="91"/>
+      <c r="AC14" s="91"/>
+      <c r="AD14" s="91"/>
+      <c r="AE14" s="91"/>
+      <c r="AF14" s="91"/>
+      <c r="AG14" s="91"/>
+      <c r="AH14" s="91"/>
+      <c r="AI14" s="91"/>
+      <c r="AJ14" s="91"/>
+      <c r="AK14" s="91"/>
+      <c r="AL14" s="91"/>
+    </row>
+    <row r="15" spans="1:38" s="119" customFormat="1" ht="261.75" customHeight="1" thickBot="1">
+      <c r="A15" s="129"/>
+      <c r="B15" s="144"/>
+      <c r="C15" s="145"/>
+      <c r="D15" s="146"/>
+      <c r="E15" s="147"/>
+      <c r="F15" s="148"/>
+      <c r="G15" s="149"/>
+      <c r="H15" s="149"/>
+      <c r="I15" s="68">
         <v>2</v>
       </c>
-      <c r="J15" s="158"/>
-      <c r="K15" s="159"/>
-      <c r="L15" s="160"/>
-      <c r="M15" s="160"/>
-      <c r="N15" s="161"/>
-      <c r="O15" s="161"/>
-      <c r="P15" s="162"/>
-      <c r="Q15" s="162"/>
-      <c r="R15" s="162"/>
-      <c r="S15" s="163"/>
-      <c r="T15" s="164"/>
-      <c r="U15" s="165">
+      <c r="J15" s="150"/>
+      <c r="K15" s="151"/>
+      <c r="L15" s="152"/>
+      <c r="M15" s="152"/>
+      <c r="N15" s="153"/>
+      <c r="O15" s="153"/>
+      <c r="P15" s="154"/>
+      <c r="Q15" s="154"/>
+      <c r="R15" s="154"/>
+      <c r="S15" s="155"/>
+      <c r="T15" s="156"/>
+      <c r="U15" s="157">
         <v>45698</v>
       </c>
-      <c r="V15" s="35"/>
-      <c r="W15" s="35"/>
-      <c r="X15" s="35"/>
-      <c r="Y15" s="99"/>
-      <c r="Z15" s="99"/>
-      <c r="AA15" s="99"/>
-      <c r="AB15" s="99"/>
-      <c r="AC15" s="99"/>
-      <c r="AD15" s="99"/>
-      <c r="AE15" s="99"/>
-      <c r="AF15" s="99"/>
-      <c r="AG15" s="99"/>
-      <c r="AH15" s="99"/>
-      <c r="AI15" s="99"/>
-      <c r="AJ15" s="99"/>
-      <c r="AK15" s="99"/>
-      <c r="AL15" s="99"/>
+      <c r="V15" s="31"/>
+      <c r="W15" s="31"/>
+      <c r="X15" s="31"/>
+      <c r="Y15" s="91"/>
+      <c r="Z15" s="91"/>
+      <c r="AA15" s="91"/>
+      <c r="AB15" s="91"/>
+      <c r="AC15" s="91"/>
+      <c r="AD15" s="91"/>
+      <c r="AE15" s="91"/>
+      <c r="AF15" s="91"/>
+      <c r="AG15" s="91"/>
+      <c r="AH15" s="91"/>
+      <c r="AI15" s="91"/>
+      <c r="AJ15" s="91"/>
+      <c r="AK15" s="91"/>
+      <c r="AL15" s="91"/>
     </row>
     <row r="16" spans="1:38" ht="14.25"/>
     <row r="17" spans="3:20" ht="14.25"/>
     <row r="18" spans="3:20" ht="14.25"/>
     <row r="19" spans="3:20" ht="14.25"/>
-    <row r="20" spans="3:20" s="166" customFormat="1" ht="5.0999999999999996" customHeight="1">
-      <c r="C20" s="167"/>
-      <c r="M20" s="168"/>
-      <c r="S20" s="169"/>
-      <c r="T20" s="169"/>
+    <row r="20" spans="3:20" s="158" customFormat="1" ht="5.0999999999999996" customHeight="1">
+      <c r="C20" s="159"/>
+      <c r="M20" s="160"/>
+      <c r="S20" s="161"/>
+      <c r="T20" s="161"/>
     </row>
     <row r="21" spans="3:20" ht="14.25"/>
     <row r="23" spans="3:20" ht="14.1" customHeight="1"/>

</xml_diff>